<commit_message>
simulations development / pre-global removal
</commit_message>
<xml_diff>
--- a/Simulations/Results/engine_failure/engine_failure.xlsx
+++ b/Simulations/Results/engine_failure/engine_failure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -39,6 +39,12 @@
     <t>dv_h (m/s)</t>
   </si>
   <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -63,6 +69,12 @@
     <t>dv_h (m/s)</t>
   </si>
   <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -87,6 +99,12 @@
     <t>dv_h (m/s)</t>
   </si>
   <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -109,6 +127,12 @@
   </si>
   <si>
     <t>dv_h (m/s)</t>
+  </si>
+  <si>
+    <t>delta_rho (m)</t>
+  </si>
+  <si>
+    <t>delta_rhodot (m/s)</t>
   </si>
 </sst>
 </file>
@@ -154,7 +178,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:J101"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.15625" customWidth="true"/>
@@ -165,32 +189,40 @@
     <col min="6" max="6" width="16.046875" customWidth="true"/>
     <col min="7" max="7" width="16.046875" customWidth="true"/>
     <col min="8" max="8" width="16.046875" customWidth="true"/>
+    <col min="9" max="9" width="15.7109375" customWidth="true"/>
+    <col min="10" max="10" width="16.48828125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2">
@@ -201,22 +233,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>0.00094957497281278336</v>
+        <v>0.00096365356915217859</v>
       </c>
       <c r="D2" s="0">
-        <v>-0.00010772433624484101</v>
+        <v>-0.00038155754941088249</v>
       </c>
       <c r="E2" s="0">
-        <v>0.00022031616498104353</v>
+        <v>-0.0025337945885869906</v>
       </c>
       <c r="F2" s="0">
-        <v>-8.418016043607035e-07</v>
+        <v>-1.8053477508217508e-06</v>
       </c>
       <c r="G2" s="0">
-        <v>-2.1422515744233019e-06</v>
+        <v>-4.9725202727439466e-06</v>
       </c>
       <c r="H2" s="0">
-        <v>2.2054386997411127e-06</v>
+        <v>-2.5366053489421192e-05</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0.0027375772832935489</v>
+      </c>
+      <c r="J2" s="0">
+        <v>2.5911810202925302e-05</v>
       </c>
     </row>
     <row r="3">
@@ -227,22 +265,28 @@
         <v>1</v>
       </c>
       <c r="C3" s="0">
-        <v>0.0009401780508380142</v>
+        <v>0.00094133920998107357</v>
       </c>
       <c r="D3" s="0">
-        <v>5.6978105445804061e-05</v>
+        <v>5.3356916666025267e-05</v>
       </c>
       <c r="E3" s="0">
-        <v>-2.6442123487217724e-05</v>
+        <v>1.8693835550227659e-06</v>
       </c>
       <c r="F3" s="0">
-        <v>1.1111507963734724e-08</v>
+        <v>-2.0373561865349998e-10</v>
       </c>
       <c r="G3" s="0">
-        <v>-4.1604326619319038e-07</v>
+        <v>-4.5402615361529036e-07</v>
       </c>
       <c r="H3" s="0">
-        <v>-2.6470823850885643e-07</v>
+        <v>1.8713879477173823e-08</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0.00094285203685348878</v>
+      </c>
+      <c r="J3" s="0">
+        <v>4.5441170645130143e-07</v>
       </c>
     </row>
     <row r="4">
@@ -253,22 +297,28 @@
         <v>1</v>
       </c>
       <c r="C4" s="0">
-        <v>0.00093963450836387352</v>
+        <v>0.00094030814485002168</v>
       </c>
       <c r="D4" s="0">
-        <v>6.8695897997350652e-05</v>
+        <v>6.9496189998685676e-05</v>
       </c>
       <c r="E4" s="0">
-        <v>8.3084586652943339e-05</v>
+        <v>2.5645610993736612e-05</v>
       </c>
       <c r="F4" s="0">
-        <v>7.0945571813141317e-08</v>
+        <v>7.8008003584484342e-08</v>
       </c>
       <c r="G4" s="0">
-        <v>-2.9362922528445787e-07</v>
+        <v>-2.8591076559362702e-07</v>
       </c>
       <c r="H4" s="0">
-        <v>8.3173441832828068e-07</v>
+        <v>2.5672787343398608e-07</v>
+      </c>
+      <c r="I4" s="0">
+        <v>0.00094322151431085622</v>
+      </c>
+      <c r="J4" s="0">
+        <v>3.9209618144469048e-07</v>
       </c>
     </row>
     <row r="5">
@@ -279,22 +329,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="0">
-        <v>0.00095277153416351013</v>
+        <v>0.00094199112173676269</v>
       </c>
       <c r="D5" s="0">
-        <v>-0.00015792933435126999</v>
+        <v>4.9608721004124057e-05</v>
       </c>
       <c r="E5" s="0">
-        <v>-0.00090535297985214734</v>
+        <v>1.1622589383682191e-05</v>
       </c>
       <c r="F5" s="0">
-        <v>-1.2113913791800268e-06</v>
+        <v>-9.9996630351095739e-09</v>
       </c>
       <c r="G5" s="0">
-        <v>-2.6778576200374611e-06</v>
+        <v>-4.9311913544441283e-07</v>
       </c>
       <c r="H5" s="0">
-        <v>-9.0634547283456045e-06</v>
+        <v>1.1633262112733989e-07</v>
+      </c>
+      <c r="I5" s="0">
+        <v>0.00094336810589214389</v>
+      </c>
+      <c r="J5" s="0">
+        <v>5.0675413539567495e-07</v>
       </c>
     </row>
     <row r="6">
@@ -305,22 +361,28 @@
         <v>1</v>
       </c>
       <c r="C6" s="0">
-        <v>0.00093996839143262179</v>
+        <v>0.00094001343736138665</v>
       </c>
       <c r="D6" s="0">
-        <v>7.0068994482586078e-05</v>
+        <v>6.6529722631658572e-05</v>
       </c>
       <c r="E6" s="0">
-        <v>0.00019106709569406523</v>
+        <v>1.4483690039863523e-05</v>
       </c>
       <c r="F6" s="0">
-        <v>1.0572642654416153e-07</v>
+        <v>5.8635260397066347e-08</v>
       </c>
       <c r="G6" s="0">
-        <v>-2.7753471436471611e-07</v>
+        <v>-3.1671408964092235e-07</v>
       </c>
       <c r="H6" s="0">
-        <v>1.9126968357269829e-06</v>
+        <v>1.4499006003391031e-07</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0.00094247612367135639</v>
+      </c>
+      <c r="J6" s="0">
+        <v>3.5322517725602018e-07</v>
       </c>
     </row>
     <row r="7">
@@ -331,22 +393,28 @@
         <v>1</v>
       </c>
       <c r="C7" s="0">
-        <v>0.00094026989772633129</v>
+        <v>0.00093981561555178672</v>
       </c>
       <c r="D7" s="0">
-        <v>6.9455987695254962e-05</v>
+        <v>7.1135921968334959e-05</v>
       </c>
       <c r="E7" s="0">
-        <v>0.00010571006950153738</v>
+        <v>3.2546230388706373e-05</v>
       </c>
       <c r="F7" s="0">
-        <v>7.7588371810710655e-08</v>
+        <v>8.9047247353590819e-08</v>
       </c>
       <c r="G7" s="0">
-        <v>-2.8626549797945364e-07</v>
+        <v>-2.6809487507209115e-07</v>
       </c>
       <c r="H7" s="0">
-        <v>1.0582312084371785e-06</v>
+        <v>3.2580723910987507e-07</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0.00094306572821929203</v>
+      </c>
+      <c r="J7" s="0">
+        <v>4.3122457183881702e-07</v>
       </c>
     </row>
     <row r="8">
@@ -357,22 +425,28 @@
         <v>1</v>
       </c>
       <c r="C8" s="0">
-        <v>0.0009397033862246218</v>
+        <v>0.00094069894839954316</v>
       </c>
       <c r="D8" s="0">
-        <v>6.8777664934627225e-05</v>
+        <v>6.7667570831542179e-05</v>
       </c>
       <c r="E8" s="0">
-        <v>8.3969143906456367e-05</v>
+        <v>1.8395655498219258e-05</v>
       </c>
       <c r="F8" s="0">
-        <v>7.1655087752198199e-08</v>
+        <v>6.5882651154036687e-08</v>
       </c>
       <c r="G8" s="0">
-        <v>-2.9283436310317476e-07</v>
+        <v>-3.0557312939499467e-07</v>
       </c>
       <c r="H8" s="0">
-        <v>8.4058958972316653e-07</v>
+        <v>1.8415135045494073e-07</v>
+      </c>
+      <c r="I8" s="0">
+        <v>0.00094330896942807516</v>
+      </c>
+      <c r="J8" s="0">
+        <v>3.6280460444392522e-07</v>
       </c>
     </row>
     <row r="9">
@@ -383,22 +457,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="0">
-        <v>0.00093958826153706099</v>
+        <v>0.00094023044092494956</v>
       </c>
       <c r="D9" s="0">
-        <v>6.8632823782555086e-05</v>
+        <v>6.9003839069825545e-05</v>
       </c>
       <c r="E9" s="0">
-        <v>8.3094620741511755e-05</v>
+        <v>4.3467183470782338e-05</v>
       </c>
       <c r="F9" s="0">
-        <v>7.046976713276365e-08</v>
+        <v>7.7116884440731059e-08</v>
       </c>
       <c r="G9" s="0">
-        <v>-2.9424616972573842e-07</v>
+        <v>-2.908204490155962e-07</v>
       </c>
       <c r="H9" s="0">
-        <v>8.3183473754074047e-07</v>
+        <v>4.3512581933847662e-07</v>
+      </c>
+      <c r="I9" s="0">
+        <v>0.00094376067299246056</v>
+      </c>
+      <c r="J9" s="0">
+        <v>5.2901609246454746e-07</v>
       </c>
     </row>
     <row r="10">
@@ -409,22 +489,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="0">
-        <v>0.00093970996478809354</v>
+        <v>0.00094081044185312379</v>
       </c>
       <c r="D10" s="0">
-        <v>6.8794359801171989e-05</v>
+        <v>6.7239059475920904e-05</v>
       </c>
       <c r="E10" s="0">
-        <v>8.6685461493842951e-05</v>
+        <v>2.1320422945508215e-05</v>
       </c>
       <c r="F10" s="0">
-        <v>7.1747269528299462e-08</v>
+        <v>6.6827594707996596e-08</v>
       </c>
       <c r="G10" s="0">
-        <v>-2.9267591288625189e-07</v>
+        <v>-3.0993229931716021e-07</v>
       </c>
       <c r="H10" s="0">
-        <v>8.6778155436673316e-07</v>
+        <v>2.1343108540451272e-07</v>
+      </c>
+      <c r="I10" s="0">
+        <v>0.00094345107931129732</v>
+      </c>
+      <c r="J10" s="0">
+        <v>3.8219992908349217e-07</v>
       </c>
     </row>
     <row r="11">
@@ -435,22 +521,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="0">
-        <v>0.00093980153142148026</v>
+        <v>0.00094018607836865442</v>
       </c>
       <c r="D11" s="0">
-        <v>6.8887772274983661e-05</v>
+        <v>6.9186390456166258e-05</v>
       </c>
       <c r="E11" s="0">
-        <v>8.5859259605639183e-05</v>
+        <v>2.5296903076729177e-05</v>
       </c>
       <c r="F11" s="0">
-        <v>7.266713947240433e-08</v>
+        <v>7.6680682380148024e-08</v>
       </c>
       <c r="G11" s="0">
-        <v>-2.9176698551234767e-07</v>
+        <v>-2.8897522595400932e-07</v>
       </c>
       <c r="H11" s="0">
-        <v>8.5951111469469922e-07</v>
+        <v>2.532372882725965e-07</v>
+      </c>
+      <c r="I11" s="0">
+        <v>0.00094306762848051157</v>
+      </c>
+      <c r="J11" s="0">
+        <v>3.9181083756975637e-07</v>
       </c>
     </row>
     <row r="12">
@@ -461,22 +553,28 @@
         <v>1</v>
       </c>
       <c r="C12" s="0">
-        <v>0.00093976799569439606</v>
+        <v>0.00094362127653369043</v>
       </c>
       <c r="D12" s="0">
-        <v>6.8850234854700432e-05</v>
+        <v>1.4715609041038302e-05</v>
       </c>
       <c r="E12" s="0">
-        <v>8.547675442718917e-05</v>
+        <v>9.3578405957387055e-05</v>
       </c>
       <c r="F12" s="0">
-        <v>7.2323005279040231e-08</v>
+        <v>-1.9917502224603423e-07</v>
       </c>
       <c r="G12" s="0">
-        <v>-2.9213142213255217e-07</v>
+        <v>-8.59695689903444e-07</v>
       </c>
       <c r="H12" s="0">
-        <v>8.556819049237264e-07</v>
+        <v>9.3673460684382569e-07</v>
+      </c>
+      <c r="I12" s="0">
+        <v>0.00094836416040361079</v>
+      </c>
+      <c r="J12" s="0">
+        <v>1.2869417595152174e-06</v>
       </c>
     </row>
     <row r="13">
@@ -487,22 +585,28 @@
         <v>1</v>
       </c>
       <c r="C13" s="0">
-        <v>0.00093975766461085186</v>
+        <v>0.0009402228798229828</v>
       </c>
       <c r="D13" s="0">
-        <v>6.8841891486814966e-05</v>
+        <v>6.6210412694500675e-05</v>
       </c>
       <c r="E13" s="0">
-        <v>8.4705734844033289e-05</v>
+        <v>1.6086195564514196e-05</v>
       </c>
       <c r="F13" s="0">
-        <v>7.2214498894607182e-08</v>
+        <v>6.0564605740276445e-08</v>
       </c>
       <c r="G13" s="0">
-        <v>-2.9221007875456645e-07</v>
+        <v>-3.2000896878128099e-07</v>
       </c>
       <c r="H13" s="0">
-        <v>8.4796347350557282e-07</v>
+        <v>1.610332160803649e-07</v>
+      </c>
+      <c r="I13" s="0">
+        <v>0.00094268852129403757</v>
+      </c>
+      <c r="J13" s="0">
+        <v>3.6332562289235737e-07</v>
       </c>
     </row>
     <row r="14">
@@ -513,22 +617,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="0">
-        <v>0.00094015795187907258</v>
+        <v>0.00093999059250204908</v>
       </c>
       <c r="D14" s="0">
-        <v>6.9173055669224937e-05</v>
+        <v>6.6142893183740448e-05</v>
       </c>
       <c r="E14" s="0">
-        <v>9.579534579004494e-05</v>
+        <v>1.4425899178065175e-05</v>
       </c>
       <c r="F14" s="0">
-        <v>7.6305455266878486e-08</v>
+        <v>5.824730448661386e-08</v>
       </c>
       <c r="G14" s="0">
-        <v>-2.8904228346979949e-07</v>
+        <v>-3.2059136743185432e-07</v>
       </c>
       <c r="H14" s="0">
-        <v>9.5897881495706386e-07</v>
+        <v>1.4441215355984445e-07</v>
+      </c>
+      <c r="I14" s="0">
+        <v>0.00094242522402478417</v>
+      </c>
+      <c r="J14" s="0">
+        <v>3.5640769274466371e-07</v>
       </c>
     </row>
     <row r="15">
@@ -539,22 +649,28 @@
         <v>1</v>
       </c>
       <c r="C15" s="0">
-        <v>0.00094056316976320886</v>
+        <v>0.0009394890275924439</v>
       </c>
       <c r="D15" s="0">
-        <v>6.9107692817538258e-05</v>
+        <v>7.3932334732018656e-05</v>
       </c>
       <c r="E15" s="0">
-        <v>0.00013711413316698764</v>
+        <v>3.8990223220514661e-05</v>
       </c>
       <c r="F15" s="0">
-        <v>8.0487647942384388e-08</v>
+        <v>1.0213319004415133e-07</v>
       </c>
       <c r="G15" s="0">
-        <v>-2.8986287956347945e-07</v>
+        <v>-2.3870718070815103e-07</v>
       </c>
       <c r="H15" s="0">
-        <v>1.3726024970791822e-06</v>
+        <v>3.9031239231695258e-07</v>
+      </c>
+      <c r="I15" s="0">
+        <v>0.00094319979887206749</v>
+      </c>
+      <c r="J15" s="0">
+        <v>4.6878147385152851e-07</v>
       </c>
     </row>
     <row r="16">
@@ -565,22 +681,28 @@
         <v>1</v>
       </c>
       <c r="C16" s="0">
-        <v>0.00094000112314773787</v>
+        <v>0.0009410625612273904</v>
       </c>
       <c r="D16" s="0">
-        <v>6.9152814814343877e-05</v>
+        <v>5.1791616236529503e-05</v>
       </c>
       <c r="E16" s="0">
-        <v>9.6517154002989625e-05</v>
+        <v>9.9335400301956506e-06</v>
       </c>
       <c r="F16" s="0">
-        <v>7.4792541673862623e-08</v>
+        <v>-3.2739495073319524e-09</v>
       </c>
       <c r="G16" s="0">
-        <v>-2.8919890087157271e-07</v>
+        <v>-4.6966300371086359e-07</v>
       </c>
       <c r="H16" s="0">
-        <v>9.6620361897084498e-07</v>
+        <v>9.9437186798738668e-08</v>
+      </c>
+      <c r="I16" s="0">
+        <v>0.00094253901291871172</v>
+      </c>
+      <c r="J16" s="0">
+        <v>4.8008521110166936e-07</v>
       </c>
     </row>
     <row r="17">
@@ -591,22 +713,28 @@
         <v>1</v>
       </c>
       <c r="C17" s="0">
-        <v>0.00094008644412557629</v>
+        <v>0.00094644748169248061</v>
       </c>
       <c r="D17" s="0">
-        <v>6.9039032473350304e-05</v>
+        <v>-6.0223978528339828e-05</v>
       </c>
       <c r="E17" s="0">
-        <v>9.2623054800432215e-05</v>
+        <v>-0.00023678265892689964</v>
       </c>
       <c r="F17" s="0">
-        <v>7.5530120720312954e-08</v>
+        <v>-9.9712541973967506e-07</v>
       </c>
       <c r="G17" s="0">
-        <v>-2.9035429686052536e-07</v>
+        <v>-1.677341279150181e-06</v>
       </c>
       <c r="H17" s="0">
-        <v>9.2722206379899187e-07</v>
+        <v>-2.3705499491338954e-06</v>
+      </c>
+      <c r="I17" s="0">
+        <v>0.00097747418930645581</v>
+      </c>
+      <c r="J17" s="0">
+        <v>3.0703810725658962e-06</v>
       </c>
     </row>
     <row r="18">
@@ -617,22 +745,28 @@
         <v>1</v>
       </c>
       <c r="C18" s="0">
-        <v>0.00099346196356631111</v>
+        <v>0.00094128764254186592</v>
       </c>
       <c r="D18" s="0">
-        <v>-0.00094343828567328147</v>
+        <v>5.560921248881634e-05</v>
       </c>
       <c r="E18" s="0">
-        <v>-0.00073260863935448314</v>
+        <v>-9.7470297494841245e-06</v>
       </c>
       <c r="F18" s="0">
-        <v>1.937258650214907e-05</v>
+        <v>6.370246059816953e-09</v>
       </c>
       <c r="G18" s="0">
-        <v>-8.7016056856763745e-06</v>
+        <v>-4.3137806079356425e-07</v>
       </c>
       <c r="H18" s="0">
-        <v>-7.3398401982033437e-06</v>
+        <v>-9.7575991091849441e-08</v>
+      </c>
+      <c r="I18" s="0">
+        <v>0.00094297922305032109</v>
+      </c>
+      <c r="J18" s="0">
+        <v>4.4232192507995271e-07</v>
       </c>
     </row>
     <row r="19">
@@ -643,22 +777,28 @@
         <v>1</v>
       </c>
       <c r="C19" s="0">
-        <v>0.00093977387234822629</v>
+        <v>0.000939990548475933</v>
       </c>
       <c r="D19" s="0">
-        <v>6.8857099800700983e-05</v>
+        <v>6.6415850979273383e-05</v>
       </c>
       <c r="E19" s="0">
-        <v>8.6402385393070434e-05</v>
+        <v>1.4378812840523089e-05</v>
       </c>
       <c r="F19" s="0">
-        <v>7.2389318608867548e-08</v>
+        <v>5.8362549557045007e-08</v>
       </c>
       <c r="G19" s="0">
-        <v>-2.920666877159403e-07</v>
+        <v>-3.1784893318080945e-07</v>
       </c>
       <c r="H19" s="0">
-        <v>8.6494806788402081e-07</v>
+        <v>1.4394032257545654e-07</v>
+      </c>
+      <c r="I19" s="0">
+        <v>0.00094244365706608118</v>
+      </c>
+      <c r="J19" s="0">
+        <v>3.5376962557306087e-07</v>
       </c>
     </row>
     <row r="20">
@@ -669,22 +809,28 @@
         <v>1</v>
       </c>
       <c r="C20" s="0">
-        <v>0.00094027556428777359</v>
+        <v>0.00096060708237555303</v>
       </c>
       <c r="D20" s="0">
-        <v>6.9446988709420676e-05</v>
+        <v>-0.00033927261831989686</v>
       </c>
       <c r="E20" s="0">
-        <v>0.00010744796946646578</v>
+        <v>-0.0026046763096957358</v>
       </c>
       <c r="F20" s="0">
-        <v>7.764876973348489e-08</v>
+        <v>-1.5448085165167824e-06</v>
       </c>
       <c r="G20" s="0">
-        <v>-2.8635975434518693e-07</v>
+        <v>-4.5252465189233454e-06</v>
       </c>
       <c r="H20" s="0">
-        <v>1.0756286598015748e-06</v>
+        <v>-2.6075511930603828e-05</v>
+      </c>
+      <c r="I20" s="0">
+        <v>0.0027968215092389983</v>
+      </c>
+      <c r="J20" s="0">
+        <v>2.6510311425043524e-05</v>
       </c>
     </row>
     <row r="21">
@@ -695,22 +841,28 @@
         <v>1</v>
       </c>
       <c r="C21" s="0">
-        <v>0.00093974355789328001</v>
+        <v>0.00094368412800882595</v>
       </c>
       <c r="D21" s="0">
-        <v>6.8841062792424079e-05</v>
+        <v>1.0151012077186383e-05</v>
       </c>
       <c r="E21" s="0">
-        <v>8.6560100143339894e-05</v>
+        <v>4.4897213637761907e-05</v>
       </c>
       <c r="F21" s="0">
-        <v>7.2092181203908812e-08</v>
+        <v>-2.4635278805806848e-07</v>
       </c>
       <c r="G21" s="0">
-        <v>-2.9221859607639691e-07</v>
+        <v>-9.0918371348008495e-07</v>
       </c>
       <c r="H21" s="0">
-        <v>8.66526720460079e-07</v>
+        <v>4.4943985288222762e-07</v>
+      </c>
+      <c r="I21" s="0">
+        <v>0.00094480608396347882</v>
+      </c>
+      <c r="J21" s="0">
+        <v>1.0436957901612035e-06</v>
       </c>
     </row>
     <row r="22">
@@ -721,22 +873,28 @@
         <v>1</v>
       </c>
       <c r="C22" s="0">
-        <v>0.0009405293224356015</v>
+        <v>0.00094106710107233482</v>
       </c>
       <c r="D22" s="0">
-        <v>6.1553050389129282e-05</v>
+        <v>6.82723928812079e-05</v>
       </c>
       <c r="E22" s="0">
-        <v>4.1300739805578039e-05</v>
+        <v>2.0756192253502092e-05</v>
       </c>
       <c r="F22" s="0">
-        <v>3.134315754160788e-08</v>
+        <v>6.9771182220623729e-08</v>
       </c>
       <c r="G22" s="0">
-        <v>-3.6916232570198895e-07</v>
+        <v>-2.9964999165082648e-07</v>
       </c>
       <c r="H22" s="0">
-        <v>4.1345036141869217e-07</v>
+        <v>2.0778182701925272e-07</v>
+      </c>
+      <c r="I22" s="0">
+        <v>0.00094376863047426957</v>
+      </c>
+      <c r="J22" s="0">
+        <v>3.7125654607597496e-07</v>
       </c>
     </row>
     <row r="23">
@@ -747,22 +905,28 @@
         <v>1</v>
       </c>
       <c r="C23" s="0">
-        <v>0.00093971376693335884</v>
+        <v>0.00093998334591560706</v>
       </c>
       <c r="D23" s="0">
-        <v>6.8787702584283128e-05</v>
+        <v>6.6345426079972292e-05</v>
       </c>
       <c r="E23" s="0">
-        <v>8.444849578287095e-05</v>
+        <v>1.4334220682675864e-05</v>
       </c>
       <c r="F23" s="0">
-        <v>7.1763146147763024e-08</v>
+        <v>5.8262032399947206e-08</v>
       </c>
       <c r="G23" s="0">
-        <v>-2.9273818524062564e-07</v>
+        <v>-3.1855358047878576e-07</v>
       </c>
       <c r="H23" s="0">
-        <v>8.4538823843083102e-07</v>
+        <v>1.4349403812198797e-07</v>
+      </c>
+      <c r="I23" s="0">
+        <v>0.0009424308335591597</v>
+      </c>
+      <c r="J23" s="0">
+        <v>3.5420528938989785e-07</v>
       </c>
     </row>
     <row r="24">
@@ -773,22 +937,28 @@
         <v>1</v>
       </c>
       <c r="C24" s="0">
-        <v>0.00094019698977021449</v>
+        <v>0.00094003792346786241</v>
       </c>
       <c r="D24" s="0">
-        <v>6.9020588475077194e-05</v>
+        <v>6.6552535263608714e-05</v>
       </c>
       <c r="E24" s="0">
-        <v>9.7328883335083628e-05</v>
+        <v>1.4635002023813501e-05</v>
       </c>
       <c r="F24" s="0">
-        <v>7.6614170327338194e-08</v>
+        <v>5.8887550093145169e-08</v>
       </c>
       <c r="G24" s="0">
-        <v>-2.9058099220184361e-07</v>
+        <v>-3.1649581239351701e-07</v>
       </c>
       <c r="H24" s="0">
-        <v>9.7433095581172341e-07</v>
+        <v>1.4650482703257719e-07</v>
+      </c>
+      <c r="I24" s="0">
+        <v>0.00094250449377815783</v>
+      </c>
+      <c r="J24" s="0">
+        <v>3.5369620744708353e-07</v>
       </c>
     </row>
     <row r="25">
@@ -799,22 +969,28 @@
         <v>1</v>
       </c>
       <c r="C25" s="0">
-        <v>0.00093957247355813678</v>
+        <v>0.00094022504746504865</v>
       </c>
       <c r="D25" s="0">
-        <v>6.8602497242997718e-05</v>
+        <v>6.6883095317271657e-05</v>
       </c>
       <c r="E25" s="0">
-        <v>8.3757718541878969e-05</v>
+        <v>1.5565041144641745e-05</v>
       </c>
       <c r="F25" s="0">
-        <v>7.0307333718822029e-08</v>
+        <v>6.0873897117508236e-08</v>
       </c>
       <c r="G25" s="0">
-        <v>-2.9454587272123231e-07</v>
+        <v>-3.1325453113623461e-07</v>
       </c>
       <c r="H25" s="0">
-        <v>8.3847269768599574e-07</v>
+        <v>1.5581508894968164e-07</v>
+      </c>
+      <c r="I25" s="0">
+        <v>0.00094272941973065985</v>
+      </c>
+      <c r="J25" s="0">
+        <v>3.5512304145472221e-07</v>
       </c>
     </row>
     <row r="26">
@@ -825,22 +1001,28 @@
         <v>1</v>
       </c>
       <c r="C26" s="0">
-        <v>0.00094030593324401224</v>
+        <v>0.00093999347835538316</v>
       </c>
       <c r="D26" s="0">
-        <v>5.4660820424934364e-05</v>
+        <v>6.6290744720975958e-05</v>
       </c>
       <c r="E26" s="0">
-        <v>2.1579753993832737e-05</v>
+        <v>1.4507753123799617e-05</v>
       </c>
       <c r="F26" s="0">
-        <v>5.2828873220445161e-09</v>
+        <v>5.8340549349833459e-08</v>
       </c>
       <c r="G26" s="0">
-        <v>-4.393668605281488e-07</v>
+        <v>-3.191080444587234e-07</v>
       </c>
       <c r="H26" s="0">
-        <v>2.1602919873265175e-07</v>
+        <v>1.4523132848488942e-07</v>
+      </c>
+      <c r="I26" s="0">
+        <v>0.00094243974719183769</v>
+      </c>
+      <c r="J26" s="0">
+        <v>3.5542327232497986e-07</v>
       </c>
     </row>
     <row r="27">
@@ -851,22 +1033,28 @@
         <v>1</v>
       </c>
       <c r="C27" s="0">
-        <v>0.00093966665359790369</v>
+        <v>0.00094000122304738198</v>
       </c>
       <c r="D27" s="0">
-        <v>6.8709912923181626e-05</v>
+        <v>6.6334538439294377e-05</v>
       </c>
       <c r="E27" s="0">
-        <v>8.8372774538723645e-05</v>
+        <v>1.4554503558850864e-05</v>
       </c>
       <c r="F27" s="0">
-        <v>7.1294782667818968e-08</v>
+        <v>5.8435554915747812e-08</v>
       </c>
       <c r="G27" s="0">
-        <v>-2.935060466769529e-07</v>
+        <v>-3.1867136092260384e-07</v>
       </c>
       <c r="H27" s="0">
-        <v>8.8467223636232317e-07</v>
+        <v>1.4569927677389727e-07</v>
+      </c>
+      <c r="I27" s="0">
+        <v>0.00094245127401599541</v>
+      </c>
+      <c r="J27" s="0">
+        <v>3.5523855309216162e-07</v>
       </c>
     </row>
     <row r="28">
@@ -877,22 +1065,28 @@
         <v>1</v>
       </c>
       <c r="C28" s="0">
-        <v>0.00092466206225694236</v>
+        <v>0.00093997850992710852</v>
       </c>
       <c r="D28" s="0">
-        <v>0.00037302986127352167</v>
+        <v>6.6293721019905494e-05</v>
       </c>
       <c r="E28" s="0">
-        <v>0.00082577989221227933</v>
+        <v>1.4321419156491175e-05</v>
       </c>
       <c r="F28" s="0">
-        <v>1.2117984503560997e-05</v>
+        <v>5.8192761734354725e-08</v>
       </c>
       <c r="G28" s="0">
-        <v>3.8050687188734278e-06</v>
+        <v>-3.1907115791065394e-07</v>
       </c>
       <c r="H28" s="0">
-        <v>8.2666042449913618e-06</v>
+        <v>1.4336596364229671e-07</v>
+      </c>
+      <c r="I28" s="0">
+        <v>0.00094242217695579946</v>
+      </c>
+      <c r="J28" s="0">
+        <v>3.5460767174414205e-07</v>
       </c>
     </row>
     <row r="29">
@@ -903,22 +1097,28 @@
         <v>1</v>
       </c>
       <c r="C29" s="0">
-        <v>0.00094156794054711668</v>
+        <v>0.0009401404916076217</v>
       </c>
       <c r="D29" s="0">
-        <v>5.6297090864576571e-05</v>
+        <v>6.6257659762591903e-05</v>
       </c>
       <c r="E29" s="0">
-        <v>5.7210033536967063e-05</v>
+        <v>1.5871041188987768e-05</v>
       </c>
       <c r="F29" s="0">
-        <v>-6.6595853553952367e-09</v>
+        <v>5.9781137227987724e-08</v>
       </c>
       <c r="G29" s="0">
-        <v>-4.2561583671330006e-07</v>
+        <v>-3.1950446358931794e-07</v>
       </c>
       <c r="H29" s="0">
-        <v>5.7274570433460832e-07</v>
+        <v>1.5887913053012256e-07</v>
+      </c>
+      <c r="I29" s="0">
+        <v>0.00094260602129726421</v>
+      </c>
+      <c r="J29" s="0">
+        <v>3.6180031058551765e-07</v>
       </c>
     </row>
     <row r="30">
@@ -929,22 +1129,28 @@
         <v>1</v>
       </c>
       <c r="C30" s="0">
-        <v>0.00094956980643257083</v>
+        <v>0.00093942252979761776</v>
       </c>
       <c r="D30" s="0">
-        <v>-0.0001089381894305852</v>
+        <v>7.3976964881594665e-05</v>
       </c>
       <c r="E30" s="0">
-        <v>-7.5283424149397737e-05</v>
+        <v>3.8787188165575542e-05</v>
       </c>
       <c r="F30" s="0">
-        <v>-1.1510146597018545e-06</v>
+        <v>1.0147271067850738e-07</v>
       </c>
       <c r="G30" s="0">
-        <v>-2.1799744644298777e-06</v>
+        <v>-2.3822285290589496e-07</v>
       </c>
       <c r="H30" s="0">
-        <v>-7.5376768201427522e-07</v>
+        <v>3.8827828729345617e-07</v>
+      </c>
+      <c r="I30" s="0">
+        <v>0.00094312869047136964</v>
+      </c>
+      <c r="J30" s="0">
+        <v>4.6669783269542552e-07</v>
       </c>
     </row>
     <row r="31">
@@ -955,22 +1161,28 @@
         <v>1</v>
       </c>
       <c r="C31" s="0">
-        <v>0.00094000560148099765</v>
+        <v>0.00094070350303354644</v>
       </c>
       <c r="D31" s="0">
-        <v>6.905001618023876e-05</v>
+        <v>6.771255259135911e-05</v>
       </c>
       <c r="E31" s="0">
-        <v>9.0592279636591121e-05</v>
+        <v>1.8306336557386327e-05</v>
       </c>
       <c r="F31" s="0">
-        <v>7.474383480893243e-08</v>
+        <v>6.5944248311966547e-08</v>
       </c>
       <c r="G31" s="0">
-        <v>-2.902161067583689e-07</v>
+        <v>-3.0512234874347302e-07</v>
       </c>
       <c r="H31" s="0">
-        <v>9.0689232345286219e-07</v>
+        <v>1.8325714192124189e-07</v>
+      </c>
+      <c r="I31" s="0">
+        <v>0.0009433150016596658</v>
+      </c>
+      <c r="J31" s="0">
+        <v>3.6198269524012616e-07</v>
       </c>
     </row>
     <row r="32">
@@ -981,22 +1193,28 @@
         <v>1</v>
       </c>
       <c r="C32" s="0">
-        <v>0.00093957646945419526</v>
+        <v>0.00094005355050441608</v>
       </c>
       <c r="D32" s="0">
-        <v>6.8617359493261532e-05</v>
+        <v>6.6074764060342073e-05</v>
       </c>
       <c r="E32" s="0">
-        <v>8.2608425483993639e-05</v>
+        <v>1.4780048125835208e-05</v>
       </c>
       <c r="F32" s="0">
-        <v>7.0344861644033863e-08</v>
+        <v>5.8835764378539768e-08</v>
       </c>
       <c r="G32" s="0">
-        <v>-2.9439600971684771e-07</v>
+        <v>-3.2130070517187581e-07</v>
       </c>
       <c r="H32" s="0">
-        <v>8.2696759600508036e-07</v>
+        <v>1.4795765783901732e-07</v>
+      </c>
+      <c r="I32" s="0">
+        <v>0.00094248872782871549</v>
+      </c>
+      <c r="J32" s="0">
+        <v>3.5859065635785806e-07</v>
       </c>
     </row>
     <row r="33">
@@ -1007,22 +1225,28 @@
         <v>1</v>
       </c>
       <c r="C33" s="0">
-        <v>0.00094104324509469706</v>
+        <v>0.00096152529812609799</v>
       </c>
       <c r="D33" s="0">
-        <v>5.923590356060604e-05</v>
+        <v>-0.00033061601522604844</v>
       </c>
       <c r="E33" s="0">
-        <v>4.3931006287300165e-05</v>
+        <v>-0.00053109346065123564</v>
       </c>
       <c r="F33" s="0">
-        <v>2.0382033304178204e-08</v>
+        <v>7.8666187429063394e-06</v>
       </c>
       <c r="G33" s="0">
-        <v>-3.9376061360249168e-07</v>
+        <v>-3.6130573587396866e-06</v>
       </c>
       <c r="H33" s="0">
-        <v>4.3978112345064682e-07</v>
+        <v>-5.3169187647720254e-06</v>
+      </c>
+      <c r="I33" s="0">
+        <v>0.0011471260228967601</v>
+      </c>
+      <c r="J33" s="0">
+        <v>1.0159109167391263e-05</v>
       </c>
     </row>
     <row r="34">
@@ -1033,22 +1257,28 @@
         <v>1</v>
       </c>
       <c r="C34" s="0">
-        <v>0.00093991806248006071</v>
+        <v>0.00094004784868406688</v>
       </c>
       <c r="D34" s="0">
-        <v>6.9018035430468139e-05</v>
+        <v>6.6433990088266004e-05</v>
       </c>
       <c r="E34" s="0">
-        <v>8.9475630776639695e-05</v>
+        <v>1.4903378895658835e-05</v>
       </c>
       <c r="F34" s="0">
-        <v>7.3877865852667313e-08</v>
+        <v>5.8939285348114101e-08</v>
       </c>
       <c r="G34" s="0">
-        <v>-2.9050737560118098e-07</v>
+        <v>-3.1769273270594589e-07</v>
       </c>
       <c r="H34" s="0">
-        <v>8.9571359186493787e-07</v>
+        <v>1.4919169952664183e-07</v>
+      </c>
+      <c r="I34" s="0">
+        <v>0.00094251023525322936</v>
+      </c>
+      <c r="J34" s="0">
+        <v>3.5589419070724625e-07</v>
       </c>
     </row>
     <row r="35">
@@ -1059,22 +1289,28 @@
         <v>1</v>
       </c>
       <c r="C35" s="0">
-        <v>0.00094035229455258218</v>
+        <v>0.00093969505869928582</v>
       </c>
       <c r="D35" s="0">
-        <v>6.9535968810763293e-05</v>
+        <v>6.85346778692697e-05</v>
       </c>
       <c r="E35" s="0">
-        <v>0.00010268414389317557</v>
+        <v>2.1571478993124651e-05</v>
       </c>
       <c r="F35" s="0">
-        <v>7.8403972363083607e-08</v>
+        <v>7.1552214979397899e-08</v>
       </c>
       <c r="G35" s="0">
-        <v>-2.8548600107102667e-07</v>
+        <v>-2.9531961526045591e-07</v>
       </c>
       <c r="H35" s="0">
-        <v>1.0279402017972276e-06</v>
+        <v>2.1594317196623836e-07</v>
+      </c>
+      <c r="I35" s="0">
+        <v>0.00094243786751193822</v>
+      </c>
+      <c r="J35" s="0">
+        <v>3.7277989235590764e-07</v>
       </c>
     </row>
     <row r="36">
@@ -1085,22 +1321,28 @@
         <v>1</v>
       </c>
       <c r="C36" s="0">
-        <v>0.00093966897968478236</v>
+        <v>0.00094014452203428078</v>
       </c>
       <c r="D36" s="0">
-        <v>6.8735359615823555e-05</v>
+        <v>6.668590090419535e-05</v>
       </c>
       <c r="E36" s="0">
-        <v>8.3537480369925962e-05</v>
+        <v>1.5295601022513403e-05</v>
       </c>
       <c r="F36" s="0">
-        <v>7.1299981148353897e-08</v>
+        <v>5.9998720089438073e-08</v>
       </c>
       <c r="G36" s="0">
-        <v>-2.9324608106021111e-07</v>
+        <v>-3.1520258637202092e-07</v>
       </c>
       <c r="H36" s="0">
-        <v>8.3626827462522016e-07</v>
+        <v>1.531179329410792e-07</v>
+      </c>
+      <c r="I36" s="0">
+        <v>0.00094263072679661277</v>
+      </c>
+      <c r="J36" s="0">
+        <v>3.5552442708783156e-07</v>
       </c>
     </row>
     <row r="37">
@@ -1111,22 +1353,28 @@
         <v>1</v>
       </c>
       <c r="C37" s="0">
-        <v>0.00094073516540227331</v>
+        <v>0.00094048468803453744</v>
       </c>
       <c r="D37" s="0">
-        <v>6.9978086458477584e-05</v>
+        <v>5.7830315458529125e-05</v>
       </c>
       <c r="E37" s="0">
-        <v>0.00011899279963854344</v>
+        <v>4.6144701567454798e-06</v>
       </c>
       <c r="F37" s="0">
-        <v>8.2410521247411328e-08</v>
+        <v>1.4286508705219081e-08</v>
       </c>
       <c r="G37" s="0">
-        <v>-2.8120865996862296e-07</v>
+        <v>-4.0768989697853239e-07</v>
       </c>
       <c r="H37" s="0">
-        <v>1.1912010351541032e-06</v>
+        <v>4.6194325794141203e-08</v>
+      </c>
+      <c r="I37" s="0">
+        <v>0.00094227229989439975</v>
+      </c>
+      <c r="J37" s="0">
+        <v>4.1054728371397844e-07</v>
       </c>
     </row>
     <row r="38">
@@ -1137,22 +1385,28 @@
         <v>1</v>
       </c>
       <c r="C38" s="0">
-        <v>0.00094005237332073222</v>
+        <v>0.00093999518152099171</v>
       </c>
       <c r="D38" s="0">
-        <v>6.9160081102248583e-05</v>
+        <v>6.636275452670537e-05</v>
       </c>
       <c r="E38" s="0">
-        <v>9.3147878929796993e-05</v>
+        <v>1.4456977436850457e-05</v>
       </c>
       <c r="F38" s="0">
-        <v>7.5266127851081333e-08</v>
+        <v>5.838697592075448e-08</v>
       </c>
       <c r="G38" s="0">
-        <v>-2.8913522156582064e-07</v>
+        <v>-3.1838489468992426e-07</v>
       </c>
       <c r="H38" s="0">
-        <v>9.3247549274077997e-07</v>
+        <v>1.4472291272554795e-07</v>
+      </c>
+      <c r="I38" s="0">
+        <v>0.00094244573353995478</v>
+      </c>
+      <c r="J38" s="0">
+        <v>3.545739719602265e-07</v>
       </c>
     </row>
     <row r="39">
@@ -1163,22 +1417,28 @@
         <v>1</v>
       </c>
       <c r="C39" s="0">
-        <v>0.00093977293429681197</v>
+        <v>0.00094016773939209486</v>
       </c>
       <c r="D39" s="0">
-        <v>6.8858984352548891e-05</v>
+        <v>6.6124293668812228e-05</v>
       </c>
       <c r="E39" s="0">
-        <v>8.4984436165359524e-05</v>
+        <v>1.535001836629687e-05</v>
       </c>
       <c r="F39" s="0">
-        <v>7.2371882819943778e-08</v>
+        <v>5.9977893526741433e-08</v>
       </c>
       <c r="G39" s="0">
-        <v>-2.9204437510628109e-07</v>
+        <v>-3.2084821518932674e-07</v>
       </c>
       <c r="H39" s="0">
-        <v>8.5075349214070798e-07</v>
+        <v>1.5366360823720112e-07</v>
+      </c>
+      <c r="I39" s="0">
+        <v>0.00094261520434941375</v>
+      </c>
+      <c r="J39" s="0">
+        <v>3.6076783309845916e-07</v>
       </c>
     </row>
     <row r="40">
@@ -1189,22 +1449,28 @@
         <v>1</v>
       </c>
       <c r="C40" s="0">
-        <v>0.00093982661208258378</v>
+        <v>0.00094013639658374615</v>
       </c>
       <c r="D40" s="0">
-        <v>6.8767357396470885e-05</v>
+        <v>6.6774019091386805e-05</v>
       </c>
       <c r="E40" s="0">
-        <v>0.00010152591497347463</v>
+        <v>1.5020636171751382e-05</v>
       </c>
       <c r="F40" s="0">
-        <v>7.2949376560271784e-08</v>
+        <v>5.994912657264484e-08</v>
       </c>
       <c r="G40" s="0">
-        <v>-2.9300220859675499e-07</v>
+        <v>-3.1431100199928383e-07</v>
       </c>
       <c r="H40" s="0">
-        <v>1.0163435347293808e-06</v>
+        <v>1.5036516503743195e-07</v>
+      </c>
+      <c r="I40" s="0">
+        <v>0.00094262443916869239</v>
+      </c>
+      <c r="J40" s="0">
+        <v>3.5354630051996151e-07</v>
       </c>
     </row>
     <row r="41">
@@ -1215,22 +1481,28 @@
         <v>1</v>
       </c>
       <c r="C41" s="0">
-        <v>0.00094074389683829196</v>
+        <v>0.00094134806073764565</v>
       </c>
       <c r="D41" s="0">
-        <v>6.8270008379833769e-05</v>
+        <v>5.3363855528676396e-05</v>
       </c>
       <c r="E41" s="0">
-        <v>8.0261939359029306e-05</v>
+        <v>1.652211254674833e-06</v>
       </c>
       <c r="F41" s="0">
-        <v>6.6551876620746242e-08</v>
+        <v>-1.2147431671660769e-10</v>
       </c>
       <c r="G41" s="0">
-        <v>-2.9951283414065069e-07</v>
+        <v>-4.5395408862199463e-07</v>
       </c>
       <c r="H41" s="0">
-        <v>8.0347718975771836e-07</v>
+        <v>1.6539852498606719e-08</v>
+      </c>
+      <c r="I41" s="0">
+        <v>0.00094286086053746118</v>
+      </c>
+      <c r="J41" s="0">
+        <v>4.5425532033572379e-07</v>
       </c>
     </row>
     <row r="42">
@@ -1241,22 +1513,28 @@
         <v>1</v>
       </c>
       <c r="C42" s="0">
-        <v>0.0009405757374842949</v>
+        <v>0.00094070300686688313</v>
       </c>
       <c r="D42" s="0">
-        <v>5.1930345264294964e-05</v>
+        <v>6.794173185387109e-05</v>
       </c>
       <c r="E42" s="0">
-        <v>3.2503695005093004e-05</v>
+        <v>1.6959866301657703e-05</v>
       </c>
       <c r="F42" s="0">
-        <v>-1.782537357303271e-08</v>
+        <v>6.6003406483383653e-08</v>
       </c>
       <c r="G42" s="0">
-        <v>-4.691876280531887e-07</v>
+        <v>-3.0280696490568929e-07</v>
       </c>
       <c r="H42" s="0">
-        <v>3.2541078494250043e-07</v>
+        <v>1.6977769799863605e-07</v>
+      </c>
+      <c r="I42" s="0">
+        <v>0.00094330581632929016</v>
+      </c>
+      <c r="J42" s="0">
+        <v>3.5337370360642597e-07</v>
       </c>
     </row>
     <row r="43">
@@ -1267,22 +1545,28 @@
         <v>1</v>
       </c>
       <c r="C43" s="0">
-        <v>0.00094176337527773768</v>
+        <v>0.0010656586805328772</v>
       </c>
       <c r="D43" s="0">
-        <v>4.6158718829569789e-05</v>
+        <v>-0.0023204547037462553</v>
       </c>
       <c r="E43" s="0">
-        <v>0.00032035897881806135</v>
+        <v>0.00097660147206072635</v>
       </c>
       <c r="F43" s="0">
-        <v>3.9115062237804477e-08</v>
+        <v>5.4259841956810773e-05</v>
       </c>
       <c r="G43" s="0">
-        <v>-5.2392580020743304e-07</v>
+        <v>-1.9127117879942212e-05</v>
       </c>
       <c r="H43" s="0">
-        <v>3.2069804897256665e-06</v>
+        <v>9.8067843420634258e-06</v>
+      </c>
+      <c r="I43" s="0">
+        <v>0.0027338414165354163</v>
+      </c>
+      <c r="J43" s="0">
+        <v>5.8362231851626685e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1293,22 +1577,28 @@
         <v>1</v>
       </c>
       <c r="C44" s="0">
-        <v>0.0009400198594873288</v>
+        <v>0.00093623634628325902</v>
       </c>
       <c r="D44" s="0">
-        <v>6.9100211594896876e-05</v>
+        <v>0.00013892374858642809</v>
       </c>
       <c r="E44" s="0">
-        <v>9.1887612572644597e-05</v>
+        <v>0.00022269278337363707</v>
       </c>
       <c r="F44" s="0">
-        <v>7.4914551360938386e-08</v>
+        <v>1.6651645596416076e-07</v>
       </c>
       <c r="G44" s="0">
-        <v>-2.897213254213736e-07</v>
+        <v>4.1981872066091178e-07</v>
       </c>
       <c r="H44" s="0">
-        <v>9.1985940034753749e-07</v>
+        <v>2.2293584794407782e-06</v>
+      </c>
+      <c r="I44" s="0">
+        <v>0.00097233244304087126</v>
+      </c>
+      <c r="J44" s="0">
+        <v>2.2746460643754508e-06</v>
       </c>
     </row>
     <row r="45">
@@ -1319,22 +1609,28 @@
         <v>1</v>
       </c>
       <c r="C45" s="0">
-        <v>0.00094053383537140434</v>
+        <v>0.0009509573847452657</v>
       </c>
       <c r="D45" s="0">
-        <v>6.9669137624961408e-05</v>
+        <v>-0.00013148215002745101</v>
       </c>
       <c r="E45" s="0">
-        <v>0.00010814605200151814</v>
+        <v>-0.00095482094848068743</v>
       </c>
       <c r="F45" s="0">
-        <v>8.0252784272205613e-08</v>
+        <v>-1.9314626595046125e-06</v>
       </c>
       <c r="G45" s="0">
-        <v>-2.8421929562779877e-07</v>
+        <v>-2.4713652164473458e-06</v>
       </c>
       <c r="H45" s="0">
-        <v>1.0826180053412711e-06</v>
+        <v>-9.5589251117066857e-06</v>
+      </c>
+      <c r="I45" s="0">
+        <v>0.0013539906007926923</v>
+      </c>
+      <c r="J45" s="0">
+        <v>1.0060379879971885e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1345,22 +1641,28 @@
         <v>1</v>
       </c>
       <c r="C46" s="0">
-        <v>0.00094024240635537382</v>
+        <v>0.00094003945239773401</v>
       </c>
       <c r="D46" s="0">
-        <v>6.9583111270365983e-05</v>
+        <v>6.6184195679996893e-05</v>
       </c>
       <c r="E46" s="0">
-        <v>0.00010215314472905471</v>
+        <v>1.4898846223837096e-05</v>
       </c>
       <c r="F46" s="0">
-        <v>7.736320391249496e-08</v>
+        <v>5.8749005805991406e-08</v>
       </c>
       <c r="G46" s="0">
-        <v>-2.8496297769468187e-07</v>
+        <v>-3.2019807003069722e-07</v>
       </c>
       <c r="H46" s="0">
-        <v>1.0226220517989111e-06</v>
+        <v>1.4914671063284723e-07</v>
+      </c>
+      <c r="I46" s="0">
+        <v>0.00094248421495579508</v>
+      </c>
+      <c r="J46" s="0">
+        <v>3.5808238022440305e-07</v>
       </c>
     </row>
     <row r="47">
@@ -1371,22 +1673,28 @@
         <v>1</v>
       </c>
       <c r="C47" s="0">
-        <v>0.00093996357024650479</v>
+        <v>0.0009400103397956272</v>
       </c>
       <c r="D47" s="0">
-        <v>6.9022929137574351e-05</v>
+        <v>6.6499162728328454e-05</v>
       </c>
       <c r="E47" s="0">
-        <v>8.9615873372036626e-05</v>
+        <v>1.4488737909382831e-05</v>
       </c>
       <c r="F47" s="0">
-        <v>7.4319207066242399e-08</v>
+        <v>5.8592473275997925e-08</v>
       </c>
       <c r="G47" s="0">
-        <v>-2.9047231115764474e-07</v>
+        <v>-3.1702009747587925e-07</v>
       </c>
       <c r="H47" s="0">
-        <v>8.9711773128992329e-07</v>
+        <v>1.4504064326171024e-07</v>
+      </c>
+      <c r="I47" s="0">
+        <v>0.00094247095503918103</v>
+      </c>
+      <c r="J47" s="0">
+        <v>3.5351323642260584e-07</v>
       </c>
     </row>
     <row r="48">
@@ -1397,22 +1705,28 @@
         <v>1</v>
       </c>
       <c r="C48" s="0">
-        <v>0.00093982582917995217</v>
+        <v>0.00094016798330009976</v>
       </c>
       <c r="D48" s="0">
-        <v>6.8911672068572294e-05</v>
+        <v>5.6970420325541671e-05</v>
       </c>
       <c r="E48" s="0">
-        <v>8.5819192234518681e-05</v>
+        <v>8.1515358185141311e-06</v>
       </c>
       <c r="F48" s="0">
-        <v>7.2912944133751711e-08</v>
+        <v>1.0901131594631686e-08</v>
       </c>
       <c r="G48" s="0">
-        <v>-2.9153526319306358e-07</v>
+        <v>-4.1616683375171951e-07</v>
       </c>
       <c r="H48" s="0">
-        <v>8.5911008545535e-07</v>
+        <v>8.1603134316365617e-08</v>
+      </c>
+      <c r="I48" s="0">
+        <v>0.00094192776429556744</v>
+      </c>
+      <c r="J48" s="0">
+        <v>4.2423194094177965e-07</v>
       </c>
     </row>
     <row r="49">
@@ -1423,22 +1737,28 @@
         <v>1</v>
       </c>
       <c r="C49" s="0">
-        <v>0.00093972858553303951</v>
+        <v>0.0009400822370206896</v>
       </c>
       <c r="D49" s="0">
-        <v>6.8815471265082362e-05</v>
+        <v>6.6397060879075376e-05</v>
       </c>
       <c r="E49" s="0">
-        <v>8.5726497432823338e-05</v>
+        <v>1.5284341839077567e-05</v>
       </c>
       <c r="F49" s="0">
-        <v>7.1928713762936525e-08</v>
+        <v>5.9265642601835644e-08</v>
       </c>
       <c r="G49" s="0">
-        <v>-2.9246788197170859e-07</v>
+        <v>-3.1807953367567199e-07</v>
       </c>
       <c r="H49" s="0">
-        <v>8.5818183518296945e-07</v>
+        <v>1.5300553722799239e-07</v>
+      </c>
+      <c r="I49" s="0">
+        <v>0.00094254803228305424</v>
+      </c>
+      <c r="J49" s="0">
+        <v>3.5790739103679884e-07</v>
       </c>
     </row>
     <row r="50">
@@ -1449,22 +1769,28 @@
         <v>1</v>
       </c>
       <c r="C50" s="0">
-        <v>0.00094033365272849778</v>
+        <v>0.00094051677435214032</v>
       </c>
       <c r="D50" s="0">
-        <v>6.8862540938074979e-05</v>
+        <v>6.7030764941689025e-05</v>
       </c>
       <c r="E50" s="0">
-        <v>0.00010611114323634912</v>
+        <v>1.8423882602195366e-05</v>
       </c>
       <c r="F50" s="0">
-        <v>7.7900058410851347e-08</v>
+        <v>6.3831780493239787e-08</v>
       </c>
       <c r="G50" s="0">
-        <v>-2.9221764763064789e-07</v>
+        <v>-3.1190006661392308e-07</v>
       </c>
       <c r="H50" s="0">
-        <v>1.0622479391588719e-06</v>
+        <v>1.8443447062987583e-07</v>
+      </c>
+      <c r="I50" s="0">
+        <v>0.0009430823748414357</v>
+      </c>
+      <c r="J50" s="0">
+        <v>3.6792964233835431e-07</v>
       </c>
     </row>
     <row r="51">
@@ -1475,22 +1801,28 @@
         <v>1</v>
       </c>
       <c r="C51" s="0">
-        <v>0.00094026845337591425</v>
+        <v>0.00093998598536781941</v>
       </c>
       <c r="D51" s="0">
-        <v>6.9119186038579805e-05</v>
+        <v>6.6376875680396186e-05</v>
       </c>
       <c r="E51" s="0">
-        <v>0.00012150203997438206</v>
+        <v>1.4350505532779827e-05</v>
       </c>
       <c r="F51" s="0">
-        <v>7.7519222228816798e-08</v>
+        <v>5.8301251167069967e-08</v>
       </c>
       <c r="G51" s="0">
-        <v>-2.8964236305998453e-07</v>
+        <v>-3.182386691304856e-07</v>
       </c>
       <c r="H51" s="0">
-        <v>1.2163167115158937e-06</v>
+        <v>1.4365700941155206e-07</v>
+      </c>
+      <c r="I51" s="0">
+        <v>0.00094243592849702388</v>
+      </c>
+      <c r="J51" s="0">
+        <v>3.539946648901071e-07</v>
       </c>
     </row>
     <row r="52">
@@ -1501,22 +1833,28 @@
         <v>1</v>
       </c>
       <c r="C52" s="0">
-        <v>0.00093954786084093911</v>
+        <v>0.00093983219811288876</v>
       </c>
       <c r="D52" s="0">
-        <v>6.8767288985971398e-05</v>
+        <v>6.8462234256383425e-05</v>
       </c>
       <c r="E52" s="0">
-        <v>8.5382235214750106e-05</v>
+        <v>2.3680665023791268e-05</v>
       </c>
       <c r="F52" s="0">
-        <v>7.0162227999714943e-08</v>
+        <v>7.2893833462372992e-08</v>
       </c>
       <c r="G52" s="0">
-        <v>-2.9289018662519498e-07</v>
+        <v>-2.9610880495235109e-07</v>
       </c>
       <c r="H52" s="0">
-        <v>8.5473441250746045e-07</v>
+        <v>2.3705797190224584e-07</v>
+      </c>
+      <c r="I52" s="0">
+        <v>0.00094261997221841689</v>
+      </c>
+      <c r="J52" s="0">
+        <v>3.862517538724655e-07</v>
       </c>
     </row>
     <row r="53">
@@ -1527,22 +1865,28 @@
         <v>1</v>
       </c>
       <c r="C53" s="0">
-        <v>0.00094808284757519345</v>
+        <v>0.00094015876186492875</v>
       </c>
       <c r="D53" s="0">
-        <v>-9.0177904227772832e-05</v>
+        <v>6.6456165090766905e-05</v>
       </c>
       <c r="E53" s="0">
-        <v>0.00018503830068364072</v>
+        <v>1.5947564003812107e-05</v>
       </c>
       <c r="F53" s="0">
-        <v>-7.7402828408540403e-07</v>
+        <v>6.0049026348596435e-08</v>
       </c>
       <c r="G53" s="0">
-        <v>-1.9597571347933912e-06</v>
+        <v>-3.1751955339651139e-07</v>
       </c>
       <c r="H53" s="0">
-        <v>1.8522813547079619e-06</v>
+        <v>1.5964491845085035e-07</v>
+      </c>
+      <c r="I53" s="0">
+        <v>0.00094263950913783725</v>
+      </c>
+      <c r="J53" s="0">
+        <v>3.6043175823130948e-07</v>
       </c>
     </row>
     <row r="54">
@@ -1553,22 +1897,28 @@
         <v>1</v>
       </c>
       <c r="C54" s="0">
-        <v>0.00093967664286331853</v>
+        <v>0.000939979706717331</v>
       </c>
       <c r="D54" s="0">
-        <v>6.8740336886363718e-05</v>
+        <v>6.6284350263678959e-05</v>
       </c>
       <c r="E54" s="0">
-        <v>8.7312214176770578e-05</v>
+        <v>1.4342013914935621e-05</v>
       </c>
       <c r="F54" s="0">
-        <v>7.1403025318772517e-08</v>
+        <v>5.8200841618338828e-08</v>
       </c>
       <c r="G54" s="0">
-        <v>-2.9320651891845406e-07</v>
+        <v>-3.1916592720029197e-07</v>
       </c>
       <c r="H54" s="0">
-        <v>8.7405561054063195e-07</v>
+        <v>1.4357214946059391e-07</v>
+      </c>
+      <c r="I54" s="0">
+        <v>0.00094242302470462481</v>
+      </c>
+      <c r="J54" s="0">
+        <v>3.547776615733298e-07</v>
       </c>
     </row>
     <row r="55">
@@ -1579,22 +1929,28 @@
         <v>1</v>
       </c>
       <c r="C55" s="0">
-        <v>0.00093975273985869023</v>
+        <v>0.00094010301845948163</v>
       </c>
       <c r="D55" s="0">
-        <v>6.8780400222567817e-05</v>
+        <v>6.9714786646024596e-05</v>
       </c>
       <c r="E55" s="0">
-        <v>9.3195385387129779e-05</v>
+        <v>2.215432528727937e-05</v>
       </c>
       <c r="F55" s="0">
-        <v>7.2192987317365453e-08</v>
+        <v>7.6022409138676306e-08</v>
       </c>
       <c r="G55" s="0">
-        <v>-2.9283961677610548e-07</v>
+        <v>-2.8361570009096532e-07</v>
       </c>
       <c r="H55" s="0">
-        <v>9.3294998914078202e-07</v>
+        <v>2.2177668043822157e-07</v>
+      </c>
+      <c r="I55" s="0">
+        <v>0.00094294467012792627</v>
+      </c>
+      <c r="J55" s="0">
+        <v>3.6797033578202161e-07</v>
       </c>
     </row>
     <row r="56">
@@ -1605,22 +1961,28 @@
         <v>1</v>
       </c>
       <c r="C56" s="0">
-        <v>0.00093980723732833837</v>
+        <v>0.00094037174535799295</v>
       </c>
       <c r="D56" s="0">
-        <v>6.8893696761662682e-05</v>
+        <v>6.7651683951175379e-05</v>
       </c>
       <c r="E56" s="0">
-        <v>8.6018557516732882e-05</v>
+        <v>1.5930509004503383e-05</v>
       </c>
       <c r="F56" s="0">
-        <v>7.2726050986959834e-08</v>
+        <v>6.2634446774956221e-08</v>
       </c>
       <c r="G56" s="0">
-        <v>-2.9170980143152642e-07</v>
+        <v>-3.0559394230064707e-07</v>
       </c>
       <c r="H56" s="0">
-        <v>8.6110580432505036e-07</v>
+        <v>1.5947312516082452e-07</v>
+      </c>
+      <c r="I56" s="0">
+        <v>0.00094293666326334465</v>
+      </c>
+      <c r="J56" s="0">
+        <v>3.5034612762554695e-07</v>
       </c>
     </row>
     <row r="57">
@@ -1631,22 +1993,28 @@
         <v>1</v>
       </c>
       <c r="C57" s="0">
-        <v>0.00094092088032571297</v>
+        <v>0.00094138809409916036</v>
       </c>
       <c r="D57" s="0">
-        <v>6.8498432315933222e-05</v>
+        <v>4.4405560690297108e-05</v>
       </c>
       <c r="E57" s="0">
-        <v>8.1614855453979174e-05</v>
+        <v>-4.4382282569696174e-06</v>
       </c>
       <c r="F57" s="0">
-        <v>6.8374689313199788e-08</v>
+        <v>-4.2921207386859006e-08</v>
       </c>
       <c r="G57" s="0">
-        <v>-2.9728411090083548e-07</v>
+        <v>-5.4732718949299444e-07</v>
       </c>
       <c r="H57" s="0">
-        <v>8.170210680631632e-07</v>
+        <v>-4.4408059191577934e-08</v>
+      </c>
+      <c r="I57" s="0">
+        <v>0.00094244527448649786</v>
+      </c>
+      <c r="J57" s="0">
+        <v>5.5080065189050809e-07</v>
       </c>
     </row>
     <row r="58">
@@ -1657,22 +2025,28 @@
         <v>1</v>
       </c>
       <c r="C58" s="0">
-        <v>0.000939599055989504</v>
+        <v>0.00094342258719226635</v>
       </c>
       <c r="D58" s="0">
-        <v>6.8646667751082191e-05</v>
+        <v>1.1073192492161432e-05</v>
       </c>
       <c r="E58" s="0">
-        <v>8.3094100993384406e-05</v>
+        <v>0.00010730914544948675</v>
       </c>
       <c r="F58" s="0">
-        <v>7.0580094518879477e-08</v>
+        <v>-2.3314393536588707e-07</v>
       </c>
       <c r="G58" s="0">
-        <v>-2.9411085748385843e-07</v>
+        <v>-8.9869088177067444e-07</v>
       </c>
       <c r="H58" s="0">
-        <v>8.3182957124011132e-07</v>
+        <v>1.0742074765956359e-06</v>
+      </c>
+      <c r="I58" s="0">
+        <v>0.00094957045358078454</v>
+      </c>
+      <c r="J58" s="0">
+        <v>1.4198320669535567e-06</v>
       </c>
     </row>
     <row r="59">
@@ -1683,22 +2057,28 @@
         <v>1</v>
       </c>
       <c r="C59" s="0">
-        <v>0.00093954496030512757</v>
+        <v>0.0009400867192139728</v>
       </c>
       <c r="D59" s="0">
-        <v>6.8571384317595019e-05</v>
+        <v>6.6306997179688132e-05</v>
       </c>
       <c r="E59" s="0">
-        <v>8.2364737113207047e-05</v>
+        <v>1.5492178194233275e-05</v>
       </c>
       <c r="F59" s="0">
-        <v>7.0017489584017767e-08</v>
+        <v>5.9273270895665586e-08</v>
       </c>
       <c r="G59" s="0">
-        <v>-2.9484581792532313e-07</v>
+        <v>-3.1898697601482479e-07</v>
       </c>
       <c r="H59" s="0">
-        <v>8.2452804555989554e-07</v>
+        <v>1.5508626080736111e-07</v>
+      </c>
+      <c r="I59" s="0">
+        <v>0.00094254955578085124</v>
+      </c>
+      <c r="J59" s="0">
+        <v>3.59607786068325e-07</v>
       </c>
     </row>
     <row r="60">
@@ -1709,22 +2089,28 @@
         <v>1</v>
       </c>
       <c r="C60" s="0">
-        <v>0.00093976834658349162</v>
+        <v>0.00094057377101286477</v>
       </c>
       <c r="D60" s="0">
-        <v>6.933657290042472e-05</v>
+        <v>6.6967133089179676e-05</v>
       </c>
       <c r="E60" s="0">
-        <v>9.3006100811306755e-05</v>
+        <v>1.9231691361857631e-05</v>
       </c>
       <c r="F60" s="0">
-        <v>7.2614571487716884e-08</v>
+        <v>6.4371085725656307e-08</v>
       </c>
       <c r="G60" s="0">
-        <v>-2.8726682271395382e-07</v>
+        <v>-3.125641897827082e-07</v>
       </c>
       <c r="H60" s="0">
-        <v>9.3105280731785344e-07</v>
+        <v>1.9252138523591983e-07</v>
+      </c>
+      <c r="I60" s="0">
+        <v>0.00094315082228887579</v>
+      </c>
+      <c r="J60" s="0">
+        <v>3.7269893102231734e-07</v>
       </c>
     </row>
     <row r="61">
@@ -1735,22 +2121,28 @@
         <v>1</v>
       </c>
       <c r="C61" s="0">
-        <v>0.00093991298196449691</v>
+        <v>0.00093956439387632429</v>
       </c>
       <c r="D61" s="0">
-        <v>6.8978728761992514e-05</v>
+        <v>7.1701712579863575e-05</v>
       </c>
       <c r="E61" s="0">
-        <v>8.7731821695654773e-05</v>
+        <v>2.3105881228490126e-05</v>
       </c>
       <c r="F61" s="0">
-        <v>7.3798130065250156e-08</v>
+        <v>8.6680657568338759e-08</v>
       </c>
       <c r="G61" s="0">
-        <v>-2.9089511283152472e-07</v>
+        <v>-2.6227818875502323e-07</v>
       </c>
       <c r="H61" s="0">
-        <v>8.7825701428970025e-07</v>
+        <v>2.3130172249503352e-07</v>
+      </c>
+      <c r="I61" s="0">
+        <v>0.00094257958156031317</v>
+      </c>
+      <c r="J61" s="0">
+        <v>3.6028304362301689e-07</v>
       </c>
     </row>
     <row r="62">
@@ -1761,22 +2153,28 @@
         <v>1</v>
       </c>
       <c r="C62" s="0">
-        <v>0.00093962516348078395</v>
+        <v>0.00094002226290523794</v>
       </c>
       <c r="D62" s="0">
-        <v>6.8682220067228794e-05</v>
+        <v>6.6194622368342948e-05</v>
       </c>
       <c r="E62" s="0">
-        <v>8.4248421286228529e-05</v>
+        <v>1.4839821190158425e-05</v>
       </c>
       <c r="F62" s="0">
-        <v>7.0858094482206813e-08</v>
+        <v>5.8585011314393753e-08</v>
       </c>
       <c r="G62" s="0">
-        <v>-2.9376618211488306e-07</v>
+        <v>-3.2008657709385255e-07</v>
       </c>
       <c r="H62" s="0">
-        <v>8.4338507735931796e-07</v>
+        <v>1.4855576936618852e-07</v>
+      </c>
+      <c r="I62" s="0">
+        <v>0.00094246687107872801</v>
+      </c>
+      <c r="J62" s="0">
+        <v>3.5770999007344851e-07</v>
       </c>
     </row>
     <row r="63">
@@ -1787,22 +2185,28 @@
         <v>1</v>
       </c>
       <c r="C63" s="0">
-        <v>0.0009405423559725179</v>
+        <v>0.00093997323584371628</v>
       </c>
       <c r="D63" s="0">
-        <v>5.445303038592586e-05</v>
+        <v>6.6223784284613618e-05</v>
       </c>
       <c r="E63" s="0">
-        <v>3.6326603802149742e-05</v>
+        <v>1.4331618520276279e-05</v>
       </c>
       <c r="F63" s="0">
-        <v>-1.8527133716084165e-09</v>
+        <v>5.8111550106654253e-08</v>
       </c>
       <c r="G63" s="0">
-        <v>-4.4272181313727635e-07</v>
+        <v>-3.197717893003646e-07</v>
       </c>
       <c r="H63" s="0">
-        <v>3.636573347519025e-07</v>
+        <v>1.4346816739478829e-07</v>
+      </c>
+      <c r="I63" s="0">
+        <v>0.00094241215452523343</v>
+      </c>
+      <c r="J63" s="0">
+        <v>3.5526618829234783e-07</v>
       </c>
     </row>
     <row r="64">
@@ -1813,22 +2217,28 @@
         <v>1</v>
       </c>
       <c r="C64" s="0">
-        <v>0.00093960597525910572</v>
+        <v>0.00094006948982183758</v>
       </c>
       <c r="D64" s="0">
-        <v>6.8655824934038545e-05</v>
+        <v>6.6526447923098697e-05</v>
       </c>
       <c r="E64" s="0">
-        <v>8.3319500507375176e-05</v>
+        <v>1.4966913420155658e-05</v>
       </c>
       <c r="F64" s="0">
-        <v>7.0652892952827173e-08</v>
+        <v>5.9191348496245855e-08</v>
       </c>
       <c r="G64" s="0">
-        <v>-2.9402192508075006e-07</v>
+        <v>-3.1677280027623406e-07</v>
       </c>
       <c r="H64" s="0">
-        <v>8.3408597678472323e-07</v>
+        <v>1.4982761818732907e-07</v>
+      </c>
+      <c r="I64" s="0">
+        <v>0.00094253934796616375</v>
+      </c>
+      <c r="J64" s="0">
+        <v>3.5538280473784739e-07</v>
       </c>
     </row>
     <row r="65">
@@ -1839,22 +2249,28 @@
         <v>1</v>
       </c>
       <c r="C65" s="0">
-        <v>0.00093958758242340679</v>
+        <v>0.00094045045374357983</v>
       </c>
       <c r="D65" s="0">
-        <v>6.8631307724609236e-05</v>
+        <v>6.6347048886028492e-05</v>
       </c>
       <c r="E65" s="0">
-        <v>8.2997905201397297e-05</v>
+        <v>1.654998500027135e-05</v>
       </c>
       <c r="F65" s="0">
-        <v>7.0461533191457093e-08</v>
+        <v>6.284720384386322e-08</v>
       </c>
       <c r="G65" s="0">
-        <v>-2.9426081482120461e-07</v>
+        <v>-3.1871935413530644e-07</v>
       </c>
       <c r="H65" s="0">
-        <v>8.3086655904557883e-07</v>
+        <v>1.6567632469776374e-07</v>
+      </c>
+      <c r="I65" s="0">
+        <v>0.00094293313063329126</v>
+      </c>
+      <c r="J65" s="0">
+        <v>3.646648355638062e-07</v>
       </c>
     </row>
     <row r="66">
@@ -1865,22 +2281,28 @@
         <v>1</v>
       </c>
       <c r="C66" s="0">
-        <v>0.00094055300437734246</v>
+        <v>0.00094020162157537612</v>
       </c>
       <c r="D66" s="0">
-        <v>6.9767150108812626e-05</v>
+        <v>7.276613891565864e-05</v>
       </c>
       <c r="E66" s="0">
-        <v>0.00010945560075497299</v>
+        <v>3.1077792590210708e-05</v>
       </c>
       <c r="F66" s="0">
-        <v>8.0494596162161702e-08</v>
+        <v>9.3440582868420385e-08</v>
       </c>
       <c r="G66" s="0">
-        <v>-2.8324724369969967e-07</v>
+        <v>-2.5185068608032934e-07</v>
       </c>
       <c r="H66" s="0">
-        <v>1.0957272627230349e-06</v>
+        <v>3.1110443965958692e-07</v>
+      </c>
+      <c r="I66" s="0">
+        <v>0.00094352521395982833</v>
+      </c>
+      <c r="J66" s="0">
+        <v>4.1103027015273256e-07</v>
       </c>
     </row>
     <row r="67">
@@ -1891,22 +2313,28 @@
         <v>1</v>
       </c>
       <c r="C67" s="0">
-        <v>0.00093961155223443171</v>
+        <v>0.00093960563997885771</v>
       </c>
       <c r="D67" s="0">
-        <v>6.8645296012970203e-05</v>
+        <v>6.9132595015231058e-05</v>
       </c>
       <c r="E67" s="0">
-        <v>8.6053225796637882e-05</v>
+        <v>1.7684428716202982e-05</v>
       </c>
       <c r="F67" s="0">
-        <v>7.071874415232049e-08</v>
+        <v>7.0861929608867502e-08</v>
       </c>
       <c r="G67" s="0">
-        <v>-2.9413324494900403e-07</v>
+        <v>-2.892614475382034e-07</v>
       </c>
       <c r="H67" s="0">
-        <v>8.6145217048868514e-07</v>
+        <v>1.7703059584345276e-07</v>
+      </c>
+      <c r="I67" s="0">
+        <v>0.00094231142059970658</v>
+      </c>
+      <c r="J67" s="0">
+        <v>3.4645841015117065e-07</v>
       </c>
     </row>
     <row r="68">
@@ -1917,22 +2345,28 @@
         <v>1</v>
       </c>
       <c r="C68" s="0">
-        <v>0.00093992621278271571</v>
+        <v>0.00094810093253894223</v>
       </c>
       <c r="D68" s="0">
-        <v>6.8985641923535734e-05</v>
+        <v>-6.6841934390549085e-05</v>
       </c>
       <c r="E68" s="0">
-        <v>8.7928463818198803e-05</v>
+        <v>-0.00035955717394976777</v>
       </c>
       <c r="F68" s="0">
-        <v>7.3930305870273383e-08</v>
+        <v>-1.0906704550478485e-06</v>
       </c>
       <c r="G68" s="0">
-        <v>-2.908303700240554e-07</v>
+        <v>-1.753070189513227e-06</v>
       </c>
       <c r="H68" s="0">
-        <v>8.802255753421907e-07</v>
+        <v>-3.5996230873383069e-06</v>
+      </c>
+      <c r="I68" s="0">
+        <v>0.0010161912141979116</v>
+      </c>
+      <c r="J68" s="0">
+        <v>4.1497112552288727e-06</v>
       </c>
     </row>
     <row r="69">
@@ -1943,22 +2377,28 @@
         <v>1</v>
       </c>
       <c r="C69" s="0">
-        <v>0.00094026937642510688</v>
+        <v>0.00094035046696561153</v>
       </c>
       <c r="D69" s="0">
-        <v>5.7950682118390606e-05</v>
+        <v>6.7176380272981895e-05</v>
       </c>
       <c r="E69" s="0">
-        <v>-5.1567448263601751e-05</v>
+        <v>1.6077065040523936e-05</v>
       </c>
       <c r="F69" s="0">
-        <v>1.2525485315606488e-08</v>
+        <v>6.2229286890147506e-08</v>
       </c>
       <c r="G69" s="0">
-        <v>-4.0639907743916792e-07</v>
+        <v>-3.1035865963834064e-07</v>
       </c>
       <c r="H69" s="0">
-        <v>-5.1623681208701426e-07</v>
+        <v>1.6094061301891254e-07</v>
+      </c>
+      <c r="I69" s="0">
+        <v>0.00094288394768886655</v>
+      </c>
+      <c r="J69" s="0">
+        <v>3.5510120061507399e-07</v>
       </c>
     </row>
     <row r="70">
@@ -1969,22 +2409,28 @@
         <v>1</v>
       </c>
       <c r="C70" s="0">
-        <v>0.00094003950683774207</v>
+        <v>0.00094078092686444847</v>
       </c>
       <c r="D70" s="0">
-        <v>6.9043730285434091e-05</v>
+        <v>6.8024025242252595e-05</v>
       </c>
       <c r="E70" s="0">
-        <v>9.0867719372807412e-05</v>
+        <v>1.8215382347374713e-05</v>
       </c>
       <c r="F70" s="0">
-        <v>7.5069430650887004e-08</v>
+        <v>6.6823779627800395e-08</v>
       </c>
       <c r="G70" s="0">
-        <v>-2.9028966100569722e-07</v>
+        <v>-3.0201984179117208e-07</v>
       </c>
       <c r="H70" s="0">
-        <v>9.0964980786523006e-07</v>
+        <v>1.8234626191005313e-07</v>
+      </c>
+      <c r="I70" s="0">
+        <v>0.00094341285793450493</v>
+      </c>
+      <c r="J70" s="0">
+        <v>3.5907041313909331e-07</v>
       </c>
     </row>
     <row r="71">
@@ -1995,22 +2441,28 @@
         <v>1</v>
       </c>
       <c r="C71" s="0">
-        <v>0.00093986135565327089</v>
+        <v>0.00093999588070214912</v>
       </c>
       <c r="D71" s="0">
-        <v>6.8964996654763411e-05</v>
+        <v>6.6291360163339696e-05</v>
       </c>
       <c r="E71" s="0">
-        <v>8.8649076215778342e-05</v>
+        <v>1.4535707104120202e-05</v>
       </c>
       <c r="F71" s="0">
-        <v>7.330048585468818e-08</v>
+        <v>5.8364698858615061e-08</v>
       </c>
       <c r="G71" s="0">
-        <v>-2.9101907905162636e-07</v>
+        <v>-3.1910296685502132e-07</v>
       </c>
       <c r="H71" s="0">
-        <v>8.8743907338544598e-07</v>
+        <v>1.4551117087983535e-07</v>
+      </c>
+      <c r="I71" s="0">
+        <v>0.00094244261732496549</v>
+      </c>
+      <c r="J71" s="0">
+        <v>3.5553711814570681e-07</v>
       </c>
     </row>
     <row r="72">
@@ -2021,22 +2473,28 @@
         <v>1</v>
       </c>
       <c r="C72" s="0">
-        <v>0.00093955362049680247</v>
+        <v>0.00094034846694768248</v>
       </c>
       <c r="D72" s="0">
-        <v>6.8575824525796136e-05</v>
+        <v>6.7439373994671037e-05</v>
       </c>
       <c r="E72" s="0">
-        <v>8.3298253660001764e-05</v>
+        <v>1.5539464234955895e-05</v>
       </c>
       <c r="F72" s="0">
-        <v>7.0108481776964826e-08</v>
+        <v>6.2312193745139854e-08</v>
       </c>
       <c r="G72" s="0">
-        <v>-2.9480527011368704e-07</v>
+        <v>-3.077141716972126e-07</v>
       </c>
       <c r="H72" s="0">
-        <v>8.3387310815963113e-07</v>
+        <v>1.5555869683957692e-07</v>
+      </c>
+      <c r="I72" s="0">
+        <v>0.00094289171350922334</v>
+      </c>
+      <c r="J72" s="0">
+        <v>3.5038454462927e-07</v>
       </c>
     </row>
     <row r="73">
@@ -2047,22 +2505,28 @@
         <v>1</v>
       </c>
       <c r="C73" s="0">
-        <v>0.00093978537986938449</v>
+        <v>0.00094001910041985326</v>
       </c>
       <c r="D73" s="0">
-        <v>6.8872769144801005e-05</v>
+        <v>6.6502999002626684e-05</v>
       </c>
       <c r="E73" s="0">
-        <v>8.511751030756841e-05</v>
+        <v>1.4566619376324623e-05</v>
       </c>
       <c r="F73" s="0">
-        <v>7.2499461281627653e-08</v>
+        <v>5.8681199358034952e-08</v>
       </c>
       <c r="G73" s="0">
-        <v>-2.9191055890857506e-07</v>
+        <v>-3.1698558459981527e-07</v>
       </c>
       <c r="H73" s="0">
-        <v>8.520856818660499e-07</v>
+        <v>1.4582030662625107e-07</v>
+      </c>
+      <c r="I73" s="0">
+        <v>0.00094248116396591626</v>
+      </c>
+      <c r="J73" s="0">
+        <v>3.5381761661448964e-07</v>
       </c>
     </row>
     <row r="74">
@@ -2073,22 +2537,28 @@
         <v>1</v>
       </c>
       <c r="C74" s="0">
-        <v>0.00094003711017887071</v>
+        <v>0.00094002546968763312</v>
       </c>
       <c r="D74" s="0">
-        <v>6.907953915896714e-05</v>
+        <v>6.6551370071776805e-05</v>
       </c>
       <c r="E74" s="0">
-        <v>0.00010552146696220796</v>
+        <v>1.4541281616268046e-05</v>
       </c>
       <c r="F74" s="0">
-        <v>7.5157271260672953e-08</v>
+        <v>5.8763244603632359e-08</v>
       </c>
       <c r="G74" s="0">
-        <v>-2.8995607535440768e-07</v>
+        <v>-3.1650179667212786e-07</v>
       </c>
       <c r="H74" s="0">
-        <v>1.0563423991814513e-06</v>
+        <v>1.4556658648792889e-07</v>
+      </c>
+      <c r="I74" s="0">
+        <v>0.00094249053968245718</v>
+      </c>
+      <c r="J74" s="0">
+        <v>3.5329327380347758e-07</v>
       </c>
     </row>
     <row r="75">
@@ -2099,22 +2569,28 @@
         <v>1</v>
       </c>
       <c r="C75" s="0">
-        <v>0.00094418653639927186</v>
+        <v>0.00093948944234334419</v>
       </c>
       <c r="D75" s="0">
-        <v>-4.7646883796215178e-06</v>
+        <v>7.2521379682610743e-05</v>
       </c>
       <c r="E75" s="0">
-        <v>0.00034247774574193462</v>
+        <v>2.3702801481159284e-05</v>
       </c>
       <c r="F75" s="0">
-        <v>-1.533078751378425e-07</v>
+        <v>8.6266770046861119e-08</v>
       </c>
       <c r="G75" s="0">
-        <v>-1.0510539824757845e-06</v>
+        <v>-2.540335770654864e-07</v>
       </c>
       <c r="H75" s="0">
-        <v>3.4283775911925397e-06</v>
+        <v>2.3727656706268518e-07</v>
+      </c>
+      <c r="I75" s="0">
+        <v>0.00094258240254299912</v>
+      </c>
+      <c r="J75" s="0">
+        <v>3.5815525009143366e-07</v>
       </c>
     </row>
     <row r="76">
@@ -2125,22 +2601,28 @@
         <v>1</v>
       </c>
       <c r="C76" s="0">
-        <v>0.00094060244373661561</v>
+        <v>0.00093998432778263918</v>
       </c>
       <c r="D76" s="0">
-        <v>7.0122870222066869e-05</v>
+        <v>6.6157762806884346e-05</v>
       </c>
       <c r="E76" s="0">
-        <v>0.00016762461977265833</v>
+        <v>1.444331161366921e-05</v>
       </c>
       <c r="F76" s="0">
-        <v>9.6641692592935868e-08</v>
+        <v>5.8192949417557038e-08</v>
       </c>
       <c r="G76" s="0">
-        <v>-2.7845236014699404e-07</v>
+        <v>-3.2043983203954712e-07</v>
       </c>
       <c r="H76" s="0">
-        <v>1.6780264192109733e-06</v>
+        <v>1.4458642065897534e-07</v>
+      </c>
+      <c r="I76" s="0">
+        <v>0.00094242028591651271</v>
+      </c>
+      <c r="J76" s="0">
+        <v>3.5633318447545926e-07</v>
       </c>
     </row>
     <row r="77">
@@ -2151,22 +2633,28 @@
         <v>1</v>
       </c>
       <c r="C77" s="0">
-        <v>0.00094070804669676988</v>
+        <v>0.00094010172743086429</v>
       </c>
       <c r="D77" s="0">
-        <v>6.8997974045970079e-05</v>
+        <v>6.6669039697098142e-05</v>
       </c>
       <c r="E77" s="0">
-        <v>0.00014683496213430334</v>
+        <v>1.4944429905223656e-05</v>
       </c>
       <c r="F77" s="0">
-        <v>8.1916111997759611e-08</v>
+        <v>5.9566596918858572e-08</v>
       </c>
       <c r="G77" s="0">
-        <v>-2.9101622049882217e-07</v>
+        <v>-3.1535264975171215e-07</v>
       </c>
       <c r="H77" s="0">
-        <v>1.4699136919059256e-06</v>
+        <v>1.4960238309458476e-07</v>
+      </c>
+      <c r="I77" s="0">
+        <v>0.0009425812191836948</v>
+      </c>
+      <c r="J77" s="0">
+        <v>3.5408522448910335e-07</v>
       </c>
     </row>
     <row r="78">
@@ -2177,22 +2665,28 @@
         <v>1</v>
       </c>
       <c r="C78" s="0">
-        <v>0.00095627746472093378</v>
+        <v>0.00094086146143457228</v>
       </c>
       <c r="D78" s="0">
-        <v>-0.00022508965706041772</v>
+        <v>5.5205832451998837e-05</v>
       </c>
       <c r="E78" s="0">
-        <v>-0.00094026168896162155</v>
+        <v>4.020398960883209e-06</v>
       </c>
       <c r="F78" s="0">
-        <v>-1.5521698084747237e-06</v>
+        <v>1.5929485785992625e-09</v>
       </c>
       <c r="G78" s="0">
-        <v>-3.3807426914516173e-06</v>
+        <v>-4.3530298884193394e-07</v>
       </c>
       <c r="H78" s="0">
-        <v>-9.4129943353409856e-06</v>
+        <v>4.0247860604872705e-08</v>
+      </c>
+      <c r="I78" s="0">
+        <v>0.00094248826897597084</v>
+      </c>
+      <c r="J78" s="0">
+        <v>4.371625782968668e-07</v>
       </c>
     </row>
     <row r="79">
@@ -2203,22 +2697,28 @@
         <v>1</v>
       </c>
       <c r="C79" s="0">
-        <v>0.00094107111827756995</v>
+        <v>0.00094002896894807009</v>
       </c>
       <c r="D79" s="0">
-        <v>6.3199393200097376e-05</v>
+        <v>6.6520359238264604e-05</v>
       </c>
       <c r="E79" s="0">
-        <v>0.00021322260717632791</v>
+        <v>1.4625733214453133e-05</v>
       </c>
       <c r="F79" s="0">
-        <v>8.3752212116927627e-08</v>
+        <v>5.8786139907340829e-08</v>
       </c>
       <c r="G79" s="0">
-        <v>-3.4921095122368573e-07</v>
+        <v>-3.1681548423416472e-07</v>
       </c>
       <c r="H79" s="0">
-        <v>2.1344817036220007e-06</v>
+        <v>1.4641207220338878e-07</v>
+      </c>
+      <c r="I79" s="0">
+        <v>0.00094249314731027084</v>
+      </c>
+      <c r="J79" s="0">
+        <v>3.5392704923843282e-07</v>
       </c>
     </row>
     <row r="80">
@@ -2229,22 +2729,28 @@
         <v>1</v>
       </c>
       <c r="C80" s="0">
-        <v>0.0009404287313961035</v>
+        <v>0.00094002552966099273</v>
       </c>
       <c r="D80" s="0">
-        <v>6.9508733912537757e-05</v>
+        <v>6.6525133932127112e-05</v>
       </c>
       <c r="E80" s="0">
-        <v>0.00012006435882589266</v>
+        <v>1.459029256173904e-05</v>
       </c>
       <c r="F80" s="0">
-        <v>7.9229760682753003e-08</v>
+        <v>5.8753793434618284e-08</v>
       </c>
       <c r="G80" s="0">
-        <v>-2.8580697687598938e-07</v>
+        <v>-3.1676585970918936e-07</v>
       </c>
       <c r="H80" s="0">
-        <v>1.2019269070257161e-06</v>
+        <v>1.460572682938615e-07</v>
+      </c>
+      <c r="I80" s="0">
+        <v>0.00094248950471406017</v>
+      </c>
+      <c r="J80" s="0">
+        <v>3.5373060899747517e-07</v>
       </c>
     </row>
     <row r="81">
@@ -2255,22 +2761,28 @@
         <v>1</v>
       </c>
       <c r="C81" s="0">
-        <v>0.00093969509738922596</v>
+        <v>0.00094077554848492895</v>
       </c>
       <c r="D81" s="0">
-        <v>6.8763930615889368e-05</v>
+        <v>6.7432979739601162e-05</v>
       </c>
       <c r="E81" s="0">
-        <v>8.4200793682826858e-05</v>
+        <v>2.02130448986573e-05</v>
       </c>
       <c r="F81" s="0">
-        <v>7.156997184482039e-08</v>
+        <v>6.6558187246379408e-08</v>
       </c>
       <c r="G81" s="0">
-        <v>-2.9296974728143521e-07</v>
+        <v>-3.0796788863269448e-07</v>
       </c>
       <c r="H81" s="0">
-        <v>8.4290853809577292e-07</v>
+        <v>2.0234516614476952e-07</v>
+      </c>
+      <c r="I81" s="0">
+        <v>0.000943405748640401</v>
+      </c>
+      <c r="J81" s="0">
+        <v>3.7445664499452831e-07</v>
       </c>
     </row>
     <row r="82">
@@ -2281,22 +2793,28 @@
         <v>1</v>
       </c>
       <c r="C82" s="0">
-        <v>0.00094002388044955865</v>
+        <v>0.00094034470642423429</v>
       </c>
       <c r="D82" s="0">
-        <v>6.9155654720376436e-05</v>
+        <v>6.7202387920239914e-05</v>
       </c>
       <c r="E82" s="0">
-        <v>9.8645276346940328e-05</v>
+        <v>1.5917021552291798e-05</v>
       </c>
       <c r="F82" s="0">
-        <v>7.5026150903045874e-08</v>
+        <v>6.2177367268767547e-08</v>
       </c>
       <c r="G82" s="0">
-        <v>-2.8918136749838189e-07</v>
+        <v>-3.1009231408422183e-07</v>
       </c>
       <c r="H82" s="0">
-        <v>9.8750755313073048e-07</v>
+        <v>1.5933840119984461e-07</v>
+      </c>
+      <c r="I82" s="0">
+        <v>0.00094287734060022777</v>
+      </c>
+      <c r="J82" s="0">
+        <v>3.5413555928698482e-07</v>
       </c>
     </row>
     <row r="83">
@@ -2307,22 +2825,28 @@
         <v>1</v>
       </c>
       <c r="C83" s="0">
-        <v>0.00094107315064118069</v>
+        <v>0.00093998643571513441</v>
       </c>
       <c r="D83" s="0">
-        <v>5.1435872582716868e-05</v>
+        <v>6.614546139549482e-05</v>
       </c>
       <c r="E83" s="0">
-        <v>4.6239034800208636e-05</v>
+        <v>1.4412459271493403e-05</v>
       </c>
       <c r="F83" s="0">
-        <v>-3.2765885490948499e-09</v>
+        <v>5.8207664785370206e-08</v>
       </c>
       <c r="G83" s="0">
-        <v>-4.7324149640660604e-07</v>
+        <v>-3.2056392823684096e-07</v>
       </c>
       <c r="H83" s="0">
-        <v>4.6288113496487086e-07</v>
+        <v>1.4427759603444251e-07</v>
+      </c>
+      <c r="I83" s="0">
+        <v>0.00094242105259481439</v>
+      </c>
+      <c r="J83" s="0">
+        <v>3.5632202997271771e-07</v>
       </c>
     </row>
     <row r="84">
@@ -2333,22 +2857,28 @@
         <v>1</v>
       </c>
       <c r="C84" s="0">
-        <v>0.00093962968680916248</v>
+        <v>0.00094118272780452372</v>
       </c>
       <c r="D84" s="0">
-        <v>6.8662035871580596e-05</v>
+        <v>5.0639535439434002e-05</v>
       </c>
       <c r="E84" s="0">
-        <v>8.6936119862993279e-05</v>
+        <v>-5.7432098916026935e-06</v>
       </c>
       <c r="F84" s="0">
-        <v>7.090614692617514e-08</v>
+        <v>-1.1477070328835826e-08</v>
       </c>
       <c r="G84" s="0">
-        <v>-2.9397165179955234e-07</v>
+        <v>-4.8243264060736715e-07</v>
       </c>
       <c r="H84" s="0">
-        <v>8.7029043157595537e-07</v>
+        <v>-5.7490386187330751e-08</v>
+      </c>
+      <c r="I84" s="0">
+        <v>0.00094256154925126498</v>
+      </c>
+      <c r="J84" s="0">
+        <v>4.859816049715242e-07</v>
       </c>
     </row>
     <row r="85">
@@ -2359,22 +2889,28 @@
         <v>1</v>
       </c>
       <c r="C85" s="0">
-        <v>0.00093965638050264033</v>
+        <v>0.0009400157770391715</v>
       </c>
       <c r="D85" s="0">
-        <v>6.8720891661766537e-05</v>
+        <v>6.6073532958232928e-05</v>
       </c>
       <c r="E85" s="0">
-        <v>8.3522197653088874e-05</v>
+        <v>1.4614871608483535e-05</v>
       </c>
       <c r="F85" s="0">
-        <v>7.117136145012859e-08</v>
+        <v>5.8464915818345897e-08</v>
       </c>
       <c r="G85" s="0">
-        <v>-2.9338686909205144e-07</v>
+        <v>-3.2129825370576237e-07</v>
       </c>
       <c r="H85" s="0">
-        <v>8.3611524589579617e-07</v>
+        <v>1.4630404775748952e-07</v>
+      </c>
+      <c r="I85" s="0">
+        <v>0.00094244838973403338</v>
+      </c>
+      <c r="J85" s="0">
+        <v>3.5784855540611661e-07</v>
       </c>
     </row>
     <row r="86">
@@ -2385,22 +2921,28 @@
         <v>1</v>
       </c>
       <c r="C86" s="0">
-        <v>0.0009567383374440297</v>
+        <v>0.00094010873805494555</v>
       </c>
       <c r="D86" s="0">
-        <v>-0.00024462166376187922</v>
+        <v>6.6506625391926644e-05</v>
       </c>
       <c r="E86" s="0">
-        <v>-0.0010219713948232797</v>
+        <v>1.5352912940763851e-05</v>
       </c>
       <c r="F86" s="0">
-        <v>-1.7389914842361187e-06</v>
+        <v>5.9573029981274672e-08</v>
       </c>
       <c r="G86" s="0">
-        <v>-3.5917893736361721e-06</v>
+        <v>-3.1698982153917366e-07</v>
       </c>
       <c r="H86" s="0">
-        <v>-1.0231027932465645e-05</v>
+        <v>1.5369186984878236e-07</v>
+      </c>
+      <c r="I86" s="0">
+        <v>0.00094258330269745975</v>
+      </c>
+      <c r="J86" s="0">
+        <v>3.5728515742779193e-07</v>
       </c>
     </row>
     <row r="87">
@@ -2411,22 +2953,28 @@
         <v>1</v>
       </c>
       <c r="C87" s="0">
-        <v>0.00093966813851853459</v>
+        <v>0.00094014133662767563</v>
       </c>
       <c r="D87" s="0">
-        <v>6.8666731828370686e-05</v>
+        <v>6.6795535082875279e-05</v>
       </c>
       <c r="E87" s="0">
-        <v>9.0918917377228679e-05</v>
+        <v>1.4954148217130841e-05</v>
       </c>
       <c r="F87" s="0">
-        <v>7.1304354032353245e-08</v>
+        <v>6.0003768342919983e-08</v>
       </c>
       <c r="G87" s="0">
-        <v>-2.939432159660034e-07</v>
+        <v>-3.1409551844423927e-07</v>
       </c>
       <c r="H87" s="0">
-        <v>9.1016075020463491e-07</v>
+        <v>1.4969955649997311e-07</v>
+      </c>
+      <c r="I87" s="0">
+        <v>0.00094262983344045505</v>
+      </c>
+      <c r="J87" s="0">
+        <v>3.5308129961581782e-07</v>
       </c>
     </row>
     <row r="88">
@@ -2437,22 +2985,28 @@
         <v>1</v>
       </c>
       <c r="C88" s="0">
-        <v>0.00093972596601421543</v>
+        <v>0.00093997647587062971</v>
       </c>
       <c r="D88" s="0">
-        <v>6.8753000717736157e-05</v>
+        <v>6.6267240627415624e-05</v>
       </c>
       <c r="E88" s="0">
-        <v>9.228256592591325e-05</v>
+        <v>1.432133608881608e-05</v>
       </c>
       <c r="F88" s="0">
-        <v>7.1912262901430157e-08</v>
+        <v>5.8161651619870192e-08</v>
       </c>
       <c r="G88" s="0">
-        <v>-2.9309899425566943e-07</v>
+        <v>-3.1933642499846343e-07</v>
       </c>
       <c r="H88" s="0">
-        <v>9.2381166665856485e-07</v>
+        <v>1.4336517137851091e-07</v>
+      </c>
+      <c r="I88" s="0">
+        <v>0.00094241828454137558</v>
+      </c>
+      <c r="J88" s="0">
+        <v>3.5484095368818439e-07</v>
       </c>
     </row>
     <row r="89">
@@ -2463,22 +3017,28 @@
         <v>1</v>
       </c>
       <c r="C89" s="0">
-        <v>0.00094006545795544127</v>
+        <v>0.000939972225008745</v>
       </c>
       <c r="D89" s="0">
-        <v>6.9043339521623892e-05</v>
+        <v>6.9271384922742207e-05</v>
       </c>
       <c r="E89" s="0">
-        <v>9.1795695301705166e-05</v>
+        <v>2.2303992415568106e-05</v>
       </c>
       <c r="F89" s="0">
-        <v>7.5325007134474653e-08</v>
+        <v>7.4573747330108908e-08</v>
       </c>
       <c r="G89" s="0">
-        <v>-2.9030325658608788e-07</v>
+        <v>-2.8802563589247834e-07</v>
       </c>
       <c r="H89" s="0">
-        <v>9.1893956084602121e-07</v>
+        <v>2.2327551083771253e-07</v>
+      </c>
+      <c r="I89" s="0">
+        <v>0.00094278511689285761</v>
+      </c>
+      <c r="J89" s="0">
+        <v>3.7198382284981552e-07</v>
       </c>
     </row>
     <row r="90">
@@ -2489,22 +3049,28 @@
         <v>1</v>
       </c>
       <c r="C90" s="0">
-        <v>0.00094029183201360667</v>
+        <v>0.00094363092466309695</v>
       </c>
       <c r="D90" s="0">
-        <v>6.9259452842085345e-05</v>
+        <v>-6.5198280501665984e-06</v>
       </c>
       <c r="E90" s="0">
-        <v>0.00010061809924260936</v>
+        <v>0.00012499866300093147</v>
       </c>
       <c r="F90" s="0">
-        <v>7.7668112469231332e-08</v>
+        <v>-2.9833851503124897e-07</v>
       </c>
       <c r="G90" s="0">
-        <v>-2.8822815638807758e-07</v>
+        <v>-1.0799897135374374e-06</v>
       </c>
       <c r="H90" s="0">
-        <v>1.007258117357815e-06</v>
+        <v>1.2512451243065776e-06</v>
+      </c>
+      <c r="I90" s="0">
+        <v>0.00095189626319802071</v>
+      </c>
+      <c r="J90" s="0">
+        <v>1.6795826898365886e-06</v>
       </c>
     </row>
     <row r="91">
@@ -2515,22 +3081,28 @@
         <v>1</v>
       </c>
       <c r="C91" s="0">
-        <v>0.00094387506058790649</v>
+        <v>0.00094084771684155299</v>
       </c>
       <c r="D91" s="0">
-        <v>3.6613406674823601e-06</v>
+        <v>6.0795009816316803e-05</v>
       </c>
       <c r="E91" s="0">
-        <v>0.00032083887391890349</v>
+        <v>4.8972834750719487e-05</v>
       </c>
       <c r="F91" s="0">
-        <v>-1.2292558182469548e-07</v>
+        <v>3.4423644941494747e-08</v>
       </c>
       <c r="G91" s="0">
-        <v>-9.6403555210422889e-07</v>
+        <v>-3.7703117366193195e-07</v>
       </c>
       <c r="H91" s="0">
-        <v>3.2117587487797063e-06</v>
+        <v>4.9023899518173641e-07</v>
+      </c>
+      <c r="I91" s="0">
+        <v>0.00094408092770061319</v>
+      </c>
+      <c r="J91" s="0">
+        <v>6.1941243581377224e-07</v>
       </c>
     </row>
     <row r="92">
@@ -2541,22 +3113,28 @@
         <v>1</v>
       </c>
       <c r="C92" s="0">
-        <v>0.00094033424281025901</v>
+        <v>0.00093956375080228582</v>
       </c>
       <c r="D92" s="0">
-        <v>6.944655675422684e-05</v>
+        <v>7.4054797250255877e-05</v>
       </c>
       <c r="E92" s="0">
-        <v>0.00011309106498898783</v>
+        <v>4.322986879351625e-05</v>
       </c>
       <c r="F92" s="0">
-        <v>7.8259278675496535e-08</v>
+        <v>1.0292326864391743e-07</v>
       </c>
       <c r="G92" s="0">
-        <v>-2.8637134573232526e-07</v>
+        <v>-2.374980983600207e-07</v>
       </c>
       <c r="H92" s="0">
-        <v>1.1321171721455175e-06</v>
+        <v>4.3275141233238869e-07</v>
+      </c>
+      <c r="I92" s="0">
+        <v>0.0009434685879102393</v>
+      </c>
+      <c r="J92" s="0">
+        <v>5.0425423233588348e-07</v>
       </c>
     </row>
     <row r="93">
@@ -2567,22 +3145,28 @@
         <v>1</v>
       </c>
       <c r="C93" s="0">
-        <v>0.00094798480071212055</v>
+        <v>0.00094004926890445262</v>
       </c>
       <c r="D93" s="0">
-        <v>-7.9886275649254657e-05</v>
+        <v>6.6574073859460015e-05</v>
       </c>
       <c r="E93" s="0">
-        <v>-0.00029359374403994346</v>
+        <v>1.469194707922127e-05</v>
       </c>
       <c r="F93" s="0">
-        <v>-1.0650685238478008e-06</v>
+        <v>5.9008686034700553e-08</v>
       </c>
       <c r="G93" s="0">
-        <v>-1.8810544641428492e-06</v>
+        <v>-3.1628430160936943e-07</v>
       </c>
       <c r="H93" s="0">
-        <v>-2.9392277378014066e-06</v>
+        <v>1.4707487903675816e-07</v>
+      </c>
+      <c r="I93" s="0">
+        <v>0.00094251821658099494</v>
+      </c>
+      <c r="J93" s="0">
+        <v>3.537637693655831e-07</v>
       </c>
     </row>
     <row r="94">
@@ -2593,22 +3177,28 @@
         <v>1</v>
       </c>
       <c r="C94" s="0">
-        <v>0.00094009214643886452</v>
+        <v>0.00094373195985131275</v>
       </c>
       <c r="D94" s="0">
-        <v>6.9482915811713841e-05</v>
+        <v>1.8490460071129977e-05</v>
       </c>
       <c r="E94" s="0">
-        <v>9.6703596733672091e-05</v>
+        <v>5.4171467583284334e-05</v>
       </c>
       <c r="F94" s="0">
-        <v>7.5829234891244823e-08</v>
+        <v>-1.9693665016806694e-07</v>
       </c>
       <c r="G94" s="0">
-        <v>-2.8591231005653528e-07</v>
+        <v>-8.2188994439142543e-07</v>
       </c>
       <c r="H94" s="0">
-        <v>9.6806859859809961e-07</v>
+        <v>5.4227466565949083e-07</v>
+      </c>
+      <c r="I94" s="0">
+        <v>0.00094546626436831083</v>
+      </c>
+      <c r="J94" s="0">
+        <v>1.0041657920320092e-06</v>
       </c>
     </row>
     <row r="95">
@@ -2619,22 +3209,28 @@
         <v>1</v>
       </c>
       <c r="C95" s="0">
-        <v>0.0009399538590759704</v>
+        <v>0.00094065421060296472</v>
       </c>
       <c r="D95" s="0">
-        <v>6.9073205991476705e-05</v>
+        <v>7.0365439682917863e-05</v>
       </c>
       <c r="E95" s="0">
-        <v>9.0968762522562725e-05</v>
+        <v>2.6790780483802498e-05</v>
       </c>
       <c r="F95" s="0">
-        <v>7.4260470772635756e-08</v>
+        <v>8.1764907775006002e-08</v>
       </c>
       <c r="G95" s="0">
-        <v>-2.8996988065679505e-07</v>
+        <v>-2.77313263467166e-07</v>
       </c>
       <c r="H95" s="0">
-        <v>9.1066083646424059e-07</v>
+        <v>2.681911151665021e-07</v>
+      </c>
+      <c r="I95" s="0">
+        <v>0.00094366274958047826</v>
+      </c>
+      <c r="J95" s="0">
+        <v>3.9435342079474481e-07</v>
       </c>
     </row>
     <row r="96">
@@ -2645,22 +3241,28 @@
         <v>1</v>
       </c>
       <c r="C96" s="0">
-        <v>0.0009407553432723148</v>
+        <v>0.00093999610678441314</v>
       </c>
       <c r="D96" s="0">
-        <v>6.9058779449793217e-05</v>
+        <v>6.6377727555355648e-05</v>
       </c>
       <c r="E96" s="0">
-        <v>0.00014899182291463524</v>
+        <v>1.4455662112911707e-05</v>
       </c>
       <c r="F96" s="0">
-        <v>8.2412363697215163e-08</v>
+        <v>5.840229350129178e-08</v>
       </c>
       <c r="G96" s="0">
-        <v>-2.9042652282184819e-07</v>
+        <v>-3.1823478883769712e-07</v>
       </c>
       <c r="H96" s="0">
-        <v>1.49150554859809e-06</v>
+        <v>1.4470972125159454e-07</v>
+      </c>
+      <c r="I96" s="0">
+        <v>0.0009424476906716837</v>
+      </c>
+      <c r="J96" s="0">
+        <v>3.5443633016029677e-07</v>
       </c>
     </row>
     <row r="97">
@@ -2671,22 +3273,28 @@
         <v>1</v>
       </c>
       <c r="C97" s="0">
-        <v>0.00094159365315338306</v>
+        <v>0.00094083970453695542</v>
       </c>
       <c r="D97" s="0">
-        <v>3.4176871553825983e-05</v>
+        <v>6.7969067300277519e-05</v>
       </c>
       <c r="E97" s="0">
-        <v>0.00027815802073611175</v>
+        <v>1.9045034124917354e-05</v>
       </c>
       <c r="F97" s="0">
-        <v>-1.273144918656488e-08</v>
+        <v>6.7394328999437203e-08</v>
       </c>
       <c r="G97" s="0">
-        <v>-6.4760258026291817e-07</v>
+        <v>-3.026013903136178e-07</v>
       </c>
       <c r="H97" s="0">
-        <v>2.7845078651712745e-06</v>
+        <v>1.9065191757069194e-07</v>
+      </c>
+      <c r="I97" s="0">
+        <v>0.0009434838933801014</v>
+      </c>
+      <c r="J97" s="0">
+        <v>3.6394745592516613e-07</v>
       </c>
     </row>
     <row r="98">
@@ -2697,22 +3305,28 @@
         <v>1</v>
       </c>
       <c r="C98" s="0">
-        <v>0.00093964207862029525</v>
+        <v>0.00094110168398398031</v>
       </c>
       <c r="D98" s="0">
-        <v>6.8702840381795749e-05</v>
+        <v>5.2190451678146843e-05</v>
       </c>
       <c r="E98" s="0">
-        <v>8.369160844125217e-05</v>
+        <v>1.0958980926034677e-05</v>
       </c>
       <c r="F98" s="0">
-        <v>7.1025964117066298e-08</v>
+        <v>-2.7541752559145927e-09</v>
       </c>
       <c r="G98" s="0">
-        <v>-2.9356344208785953e-07</v>
+        <v>-4.656977460716985e-07</v>
       </c>
       <c r="H98" s="0">
-        <v>8.3781111104152147e-07</v>
+        <v>1.0970278793908813e-07</v>
+      </c>
+      <c r="I98" s="0">
+        <v>0.00094261143750051628</v>
+      </c>
+      <c r="J98" s="0">
+        <v>4.784523778383895e-07</v>
       </c>
     </row>
     <row r="99">
@@ -2723,22 +3337,28 @@
         <v>1</v>
       </c>
       <c r="C99" s="0">
-        <v>0.00094077374757617349</v>
+        <v>0.00094054865167780832</v>
       </c>
       <c r="D99" s="0">
-        <v>7.008633762134453e-05</v>
+        <v>6.762761297379738e-05</v>
       </c>
       <c r="E99" s="0">
-        <v>0.00012006829800563113</v>
+        <v>1.6385567898504294e-05</v>
       </c>
       <c r="F99" s="0">
-        <v>8.286798129641948e-08</v>
+        <v>6.4354913516251333e-08</v>
       </c>
       <c r="G99" s="0">
-        <v>-2.8011111941539032e-07</v>
+        <v>-3.0590055017298487e-07</v>
       </c>
       <c r="H99" s="0">
-        <v>1.2019632281809465e-06</v>
+        <v>1.6402871584572435e-07</v>
+      </c>
+      <c r="I99" s="0">
+        <v>0.00094311915845498196</v>
+      </c>
+      <c r="J99" s="0">
+        <v>3.5301858465499577e-07</v>
       </c>
     </row>
     <row r="100">
@@ -2749,22 +3369,28 @@
         <v>1</v>
       </c>
       <c r="C100" s="0">
-        <v>0.00094018993596822753</v>
+        <v>0.00093999136727784816</v>
       </c>
       <c r="D100" s="0">
-        <v>6.930342363364872e-05</v>
+        <v>6.6400166716162889e-05</v>
       </c>
       <c r="E100" s="0">
-        <v>9.7191818061911992e-05</v>
+        <v>1.4421455083827133e-05</v>
       </c>
       <c r="F100" s="0">
-        <v>7.6688578952432973e-08</v>
+        <v>5.8364637053887058e-08</v>
       </c>
       <c r="G100" s="0">
-        <v>-2.8775155708942249e-07</v>
+        <v>-3.1800714373007161e-07</v>
       </c>
       <c r="H100" s="0">
-        <v>9.7295826343171612e-07</v>
+        <v>1.4436722875922844e-07</v>
+      </c>
+      <c r="I100" s="0">
+        <v>0.00094244402012191018</v>
+      </c>
+      <c r="J100" s="0">
+        <v>3.5408596563745618e-07</v>
       </c>
     </row>
     <row r="101">
@@ -2775,22 +3401,28 @@
         <v>1</v>
       </c>
       <c r="C101" s="0">
-        <v>0.0009402343698194926</v>
+        <v>0.00098514507378322236</v>
       </c>
       <c r="D101" s="0">
-        <v>6.9089853967474468e-05</v>
+        <v>-0.00079489257197440377</v>
       </c>
       <c r="E101" s="0">
-        <v>9.8889440439378079e-05</v>
+        <v>-0.0030367355499337089</v>
       </c>
       <c r="F101" s="0">
-        <v>7.7018317536092784e-08</v>
+        <v>-4.1743241409181175e-06</v>
       </c>
       <c r="G101" s="0">
-        <v>-2.8990284831791405e-07</v>
+        <v>-9.3207575611307415e-06</v>
       </c>
       <c r="H101" s="0">
-        <v>9.8995318803318957e-07</v>
+        <v>-3.0402522293398324e-05</v>
+      </c>
+      <c r="I101" s="0">
+        <v>0.0032900042275976816</v>
+      </c>
+      <c r="J101" s="0">
+        <v>3.2072026212065396e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>